<commit_message>
Aggiornamento matrice di tracciabilità
</commit_message>
<xml_diff>
--- a/NC09_Matrice_di_tracciabilità.xlsx
+++ b/NC09_Matrice_di_tracciabilità.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015F0E1D-2947-4695-9018-DEC9375989F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>Requisiti</t>
   </si>
@@ -229,12 +230,33 @@
   </si>
   <si>
     <t>Inventario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementato</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>TC_C_1</t>
+  </si>
+  <si>
+    <t>TC_I_1</t>
+  </si>
+  <si>
+    <t>TC_A_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -347,7 +369,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
@@ -362,6 +384,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,12 +400,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,16 +685,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CI10" sqref="CI10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -678,92 +703,134 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13" t="s">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13" t="s">
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13" t="s">
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13"/>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13"/>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13"/>
-      <c r="AQ2" s="8" t="s">
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="10"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="13"/>
+      <c r="BL2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12"/>
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12"/>
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="12"/>
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12"/>
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="12"/>
+      <c r="BW2" s="12"/>
+      <c r="BX2" s="12"/>
+      <c r="BY2" s="12"/>
+      <c r="BZ2" s="12"/>
+      <c r="CA2" s="12"/>
+      <c r="CB2" s="12"/>
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="12"/>
+      <c r="CE2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="CF2" s="12"/>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="12"/>
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12"/>
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12"/>
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="12"/>
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="12"/>
+      <c r="CQ2" s="12"/>
+      <c r="CR2" s="12"/>
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="12"/>
+      <c r="CU2" s="12"/>
+      <c r="CV2" s="12"/>
+      <c r="CW2" s="12"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -829,12 +896,52 @@
       <c r="BI3" s="4"/>
       <c r="BJ3" s="4"/>
       <c r="BK3" s="4"/>
+      <c r="BL3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CE3" s="5"/>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="5"/>
+      <c r="CH3" s="5"/>
+      <c r="CI3" s="5"/>
+      <c r="CJ3" s="5"/>
+      <c r="CK3" s="5"/>
+      <c r="CL3" s="5"/>
+      <c r="CM3" s="5"/>
+      <c r="CN3" s="5"/>
+      <c r="CO3" s="5"/>
+      <c r="CP3" s="5"/>
+      <c r="CQ3" s="5"/>
+      <c r="CR3" s="5"/>
+      <c r="CS3" s="5"/>
+      <c r="CT3" s="5"/>
+      <c r="CU3" s="5"/>
+      <c r="CV3" s="5"/>
+      <c r="CW3" s="5"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -896,12 +1003,52 @@
       <c r="BI4" s="4"/>
       <c r="BJ4" s="4"/>
       <c r="BK4" s="4"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="8"/>
+      <c r="BR4" s="8"/>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="8"/>
+      <c r="BY4" s="8"/>
+      <c r="BZ4" s="8"/>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+      <c r="CK4" s="5"/>
+      <c r="CL4" s="5"/>
+      <c r="CM4" s="5"/>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
@@ -977,12 +1124,52 @@
       <c r="BI5" s="4"/>
       <c r="BJ5" s="4"/>
       <c r="BK5" s="4"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO5" s="8"/>
+      <c r="BP5" s="8"/>
+      <c r="BQ5" s="8"/>
+      <c r="BR5" s="8"/>
+      <c r="BS5" s="8"/>
+      <c r="BT5" s="8"/>
+      <c r="BU5" s="8"/>
+      <c r="BV5" s="8"/>
+      <c r="BW5" s="8"/>
+      <c r="BX5" s="8"/>
+      <c r="BY5" s="8"/>
+      <c r="BZ5" s="8"/>
+      <c r="CA5" s="8"/>
+      <c r="CB5" s="8"/>
+      <c r="CC5" s="8"/>
+      <c r="CD5" s="8"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+      <c r="CK5" s="5"/>
+      <c r="CL5" s="5"/>
+      <c r="CM5" s="5"/>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1046,12 +1233,52 @@
       <c r="BI6" s="4"/>
       <c r="BJ6" s="4"/>
       <c r="BK6" s="4"/>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="8"/>
+      <c r="BN6" s="8"/>
+      <c r="BO6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP6" s="8"/>
+      <c r="BQ6" s="8"/>
+      <c r="BR6" s="8"/>
+      <c r="BS6" s="8"/>
+      <c r="BT6" s="8"/>
+      <c r="BU6" s="8"/>
+      <c r="BV6" s="8"/>
+      <c r="BW6" s="8"/>
+      <c r="BX6" s="8"/>
+      <c r="BY6" s="8"/>
+      <c r="BZ6" s="8"/>
+      <c r="CA6" s="8"/>
+      <c r="CB6" s="8"/>
+      <c r="CC6" s="8"/>
+      <c r="CD6" s="8"/>
+      <c r="CE6" s="5"/>
+      <c r="CF6" s="5"/>
+      <c r="CG6" s="5"/>
+      <c r="CH6" s="5"/>
+      <c r="CI6" s="5"/>
+      <c r="CJ6" s="5"/>
+      <c r="CK6" s="5"/>
+      <c r="CL6" s="5"/>
+      <c r="CM6" s="5"/>
+      <c r="CN6" s="5"/>
+      <c r="CO6" s="5"/>
+      <c r="CP6" s="5"/>
+      <c r="CQ6" s="5"/>
+      <c r="CR6" s="5"/>
+      <c r="CS6" s="5"/>
+      <c r="CT6" s="5"/>
+      <c r="CU6" s="5"/>
+      <c r="CV6" s="5"/>
+      <c r="CW6" s="5"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1117,12 +1344,54 @@
       <c r="BI7" s="4"/>
       <c r="BJ7" s="4"/>
       <c r="BK7" s="4"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ7" s="8"/>
+      <c r="BR7" s="8"/>
+      <c r="BS7" s="8"/>
+      <c r="BT7" s="8"/>
+      <c r="BU7" s="8"/>
+      <c r="BV7" s="8"/>
+      <c r="BW7" s="8"/>
+      <c r="BX7" s="8"/>
+      <c r="BY7" s="8"/>
+      <c r="BZ7" s="8"/>
+      <c r="CA7" s="8"/>
+      <c r="CB7" s="8"/>
+      <c r="CC7" s="8"/>
+      <c r="CD7" s="8"/>
+      <c r="CE7" s="5"/>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+      <c r="CJ7" s="5"/>
+      <c r="CK7" s="5"/>
+      <c r="CL7" s="5"/>
+      <c r="CM7" s="5"/>
+      <c r="CN7" s="5"/>
+      <c r="CO7" s="5"/>
+      <c r="CP7" s="5"/>
+      <c r="CQ7" s="5"/>
+      <c r="CR7" s="5"/>
+      <c r="CS7" s="5"/>
+      <c r="CT7" s="5"/>
+      <c r="CU7" s="5"/>
+      <c r="CV7" s="5"/>
+      <c r="CW7" s="5"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1186,12 +1455,54 @@
       <c r="BI8" s="4"/>
       <c r="BJ8" s="4"/>
       <c r="BK8" s="4"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+      <c r="BQ8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR8" s="8"/>
+      <c r="BS8" s="8"/>
+      <c r="BT8" s="8"/>
+      <c r="BU8" s="8"/>
+      <c r="BV8" s="8"/>
+      <c r="BW8" s="8"/>
+      <c r="BX8" s="8"/>
+      <c r="BY8" s="8"/>
+      <c r="BZ8" s="8"/>
+      <c r="CA8" s="8"/>
+      <c r="CB8" s="8"/>
+      <c r="CC8" s="8"/>
+      <c r="CD8" s="8"/>
+      <c r="CE8" s="5"/>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI8" s="5"/>
+      <c r="CJ8" s="5"/>
+      <c r="CK8" s="5"/>
+      <c r="CL8" s="5"/>
+      <c r="CM8" s="5"/>
+      <c r="CN8" s="5"/>
+      <c r="CO8" s="5"/>
+      <c r="CP8" s="5"/>
+      <c r="CQ8" s="5"/>
+      <c r="CR8" s="5"/>
+      <c r="CS8" s="5"/>
+      <c r="CT8" s="5"/>
+      <c r="CU8" s="5"/>
+      <c r="CV8" s="5"/>
+      <c r="CW8" s="5"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1259,12 +1570,52 @@
       <c r="BI9" s="4"/>
       <c r="BJ9" s="4"/>
       <c r="BK9" s="4"/>
+      <c r="BL9" s="8"/>
+      <c r="BM9" s="8"/>
+      <c r="BN9" s="8"/>
+      <c r="BO9" s="8"/>
+      <c r="BP9" s="8"/>
+      <c r="BQ9" s="8"/>
+      <c r="BR9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS9" s="8"/>
+      <c r="BT9" s="8"/>
+      <c r="BU9" s="8"/>
+      <c r="BV9" s="8"/>
+      <c r="BW9" s="8"/>
+      <c r="BX9" s="8"/>
+      <c r="BY9" s="8"/>
+      <c r="BZ9" s="8"/>
+      <c r="CA9" s="8"/>
+      <c r="CB9" s="8"/>
+      <c r="CC9" s="8"/>
+      <c r="CD9" s="8"/>
+      <c r="CE9" s="5"/>
+      <c r="CF9" s="5"/>
+      <c r="CG9" s="5"/>
+      <c r="CH9" s="5"/>
+      <c r="CI9" s="5"/>
+      <c r="CJ9" s="5"/>
+      <c r="CK9" s="5"/>
+      <c r="CL9" s="5"/>
+      <c r="CM9" s="5"/>
+      <c r="CN9" s="5"/>
+      <c r="CO9" s="5"/>
+      <c r="CP9" s="5"/>
+      <c r="CQ9" s="5"/>
+      <c r="CR9" s="5"/>
+      <c r="CS9" s="5"/>
+      <c r="CT9" s="5"/>
+      <c r="CU9" s="5"/>
+      <c r="CV9" s="5"/>
+      <c r="CW9" s="5"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1326,12 +1677,52 @@
       <c r="BI10" s="4"/>
       <c r="BJ10" s="4"/>
       <c r="BK10" s="4"/>
+      <c r="BL10" s="8"/>
+      <c r="BM10" s="8"/>
+      <c r="BN10" s="8"/>
+      <c r="BO10" s="8"/>
+      <c r="BP10" s="8"/>
+      <c r="BQ10" s="8"/>
+      <c r="BR10" s="8"/>
+      <c r="BS10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BT10" s="8"/>
+      <c r="BU10" s="8"/>
+      <c r="BV10" s="8"/>
+      <c r="BW10" s="8"/>
+      <c r="BX10" s="8"/>
+      <c r="BY10" s="8"/>
+      <c r="BZ10" s="8"/>
+      <c r="CA10" s="8"/>
+      <c r="CB10" s="8"/>
+      <c r="CC10" s="8"/>
+      <c r="CD10" s="8"/>
+      <c r="CE10" s="5"/>
+      <c r="CF10" s="5"/>
+      <c r="CG10" s="5"/>
+      <c r="CH10" s="5"/>
+      <c r="CI10" s="5"/>
+      <c r="CJ10" s="5"/>
+      <c r="CK10" s="5"/>
+      <c r="CL10" s="5"/>
+      <c r="CM10" s="5"/>
+      <c r="CN10" s="5"/>
+      <c r="CO10" s="5"/>
+      <c r="CP10" s="5"/>
+      <c r="CQ10" s="5"/>
+      <c r="CR10" s="5"/>
+      <c r="CS10" s="5"/>
+      <c r="CT10" s="5"/>
+      <c r="CU10" s="5"/>
+      <c r="CV10" s="5"/>
+      <c r="CW10" s="5"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1393,12 +1784,52 @@
       <c r="BI11" s="4"/>
       <c r="BJ11" s="4"/>
       <c r="BK11" s="4"/>
+      <c r="BL11" s="8"/>
+      <c r="BM11" s="8"/>
+      <c r="BN11" s="8"/>
+      <c r="BO11" s="8"/>
+      <c r="BP11" s="8"/>
+      <c r="BQ11" s="8"/>
+      <c r="BR11" s="8"/>
+      <c r="BS11" s="8"/>
+      <c r="BT11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU11" s="8"/>
+      <c r="BV11" s="8"/>
+      <c r="BW11" s="8"/>
+      <c r="BX11" s="8"/>
+      <c r="BY11" s="8"/>
+      <c r="BZ11" s="8"/>
+      <c r="CA11" s="8"/>
+      <c r="CB11" s="8"/>
+      <c r="CC11" s="8"/>
+      <c r="CD11" s="8"/>
+      <c r="CE11" s="5"/>
+      <c r="CF11" s="5"/>
+      <c r="CG11" s="5"/>
+      <c r="CH11" s="5"/>
+      <c r="CI11" s="5"/>
+      <c r="CJ11" s="5"/>
+      <c r="CK11" s="5"/>
+      <c r="CL11" s="5"/>
+      <c r="CM11" s="5"/>
+      <c r="CN11" s="5"/>
+      <c r="CO11" s="5"/>
+      <c r="CP11" s="5"/>
+      <c r="CQ11" s="5"/>
+      <c r="CR11" s="5"/>
+      <c r="CS11" s="5"/>
+      <c r="CT11" s="5"/>
+      <c r="CU11" s="5"/>
+      <c r="CV11" s="5"/>
+      <c r="CW11" s="5"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1462,12 +1893,52 @@
       <c r="BI12" s="4"/>
       <c r="BJ12" s="4"/>
       <c r="BK12" s="4"/>
+      <c r="BL12" s="8"/>
+      <c r="BM12" s="8"/>
+      <c r="BN12" s="8"/>
+      <c r="BO12" s="8"/>
+      <c r="BP12" s="8"/>
+      <c r="BQ12" s="8"/>
+      <c r="BR12" s="8"/>
+      <c r="BS12" s="8"/>
+      <c r="BT12" s="8"/>
+      <c r="BU12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV12" s="8"/>
+      <c r="BW12" s="8"/>
+      <c r="BX12" s="8"/>
+      <c r="BY12" s="8"/>
+      <c r="BZ12" s="8"/>
+      <c r="CA12" s="8"/>
+      <c r="CB12" s="8"/>
+      <c r="CC12" s="8"/>
+      <c r="CD12" s="8"/>
+      <c r="CE12" s="5"/>
+      <c r="CF12" s="5"/>
+      <c r="CG12" s="5"/>
+      <c r="CH12" s="5"/>
+      <c r="CI12" s="5"/>
+      <c r="CJ12" s="5"/>
+      <c r="CK12" s="5"/>
+      <c r="CL12" s="5"/>
+      <c r="CM12" s="5"/>
+      <c r="CN12" s="5"/>
+      <c r="CO12" s="5"/>
+      <c r="CP12" s="5"/>
+      <c r="CQ12" s="5"/>
+      <c r="CR12" s="5"/>
+      <c r="CS12" s="5"/>
+      <c r="CT12" s="5"/>
+      <c r="CU12" s="5"/>
+      <c r="CV12" s="5"/>
+      <c r="CW12" s="5"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
@@ -1541,12 +2012,54 @@
       <c r="BI13" s="4"/>
       <c r="BJ13" s="4"/>
       <c r="BK13" s="4"/>
+      <c r="BL13" s="8"/>
+      <c r="BM13" s="8"/>
+      <c r="BN13" s="8"/>
+      <c r="BO13" s="8"/>
+      <c r="BP13" s="8"/>
+      <c r="BQ13" s="8"/>
+      <c r="BR13" s="8"/>
+      <c r="BS13" s="8"/>
+      <c r="BT13" s="8"/>
+      <c r="BU13" s="8"/>
+      <c r="BV13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW13" s="8"/>
+      <c r="BX13" s="8"/>
+      <c r="BY13" s="8"/>
+      <c r="BZ13" s="8"/>
+      <c r="CA13" s="8"/>
+      <c r="CB13" s="8"/>
+      <c r="CC13" s="8"/>
+      <c r="CD13" s="8"/>
+      <c r="CE13" s="5"/>
+      <c r="CF13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG13" s="5"/>
+      <c r="CH13" s="5"/>
+      <c r="CI13" s="5"/>
+      <c r="CJ13" s="5"/>
+      <c r="CK13" s="5"/>
+      <c r="CL13" s="5"/>
+      <c r="CM13" s="5"/>
+      <c r="CN13" s="5"/>
+      <c r="CO13" s="5"/>
+      <c r="CP13" s="5"/>
+      <c r="CQ13" s="5"/>
+      <c r="CR13" s="5"/>
+      <c r="CS13" s="5"/>
+      <c r="CT13" s="5"/>
+      <c r="CU13" s="5"/>
+      <c r="CV13" s="5"/>
+      <c r="CW13" s="5"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1620,12 +2133,52 @@
       <c r="BI14" s="4"/>
       <c r="BJ14" s="4"/>
       <c r="BK14" s="4"/>
+      <c r="BL14" s="8"/>
+      <c r="BM14" s="8"/>
+      <c r="BN14" s="8"/>
+      <c r="BO14" s="8"/>
+      <c r="BP14" s="8"/>
+      <c r="BQ14" s="8"/>
+      <c r="BR14" s="8"/>
+      <c r="BS14" s="8"/>
+      <c r="BT14" s="8"/>
+      <c r="BU14" s="8"/>
+      <c r="BV14" s="8"/>
+      <c r="BW14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BX14" s="8"/>
+      <c r="BY14" s="8"/>
+      <c r="BZ14" s="8"/>
+      <c r="CA14" s="8"/>
+      <c r="CB14" s="8"/>
+      <c r="CC14" s="8"/>
+      <c r="CD14" s="8"/>
+      <c r="CE14" s="5"/>
+      <c r="CF14" s="5"/>
+      <c r="CG14" s="5"/>
+      <c r="CH14" s="5"/>
+      <c r="CI14" s="5"/>
+      <c r="CJ14" s="5"/>
+      <c r="CK14" s="5"/>
+      <c r="CL14" s="5"/>
+      <c r="CM14" s="5"/>
+      <c r="CN14" s="5"/>
+      <c r="CO14" s="5"/>
+      <c r="CP14" s="5"/>
+      <c r="CQ14" s="5"/>
+      <c r="CR14" s="5"/>
+      <c r="CS14" s="5"/>
+      <c r="CT14" s="5"/>
+      <c r="CU14" s="5"/>
+      <c r="CV14" s="5"/>
+      <c r="CW14" s="5"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1687,12 +2240,52 @@
       <c r="BI15" s="4"/>
       <c r="BJ15" s="4"/>
       <c r="BK15" s="4"/>
+      <c r="BL15" s="8"/>
+      <c r="BM15" s="8"/>
+      <c r="BN15" s="8"/>
+      <c r="BO15" s="8"/>
+      <c r="BP15" s="8"/>
+      <c r="BQ15" s="8"/>
+      <c r="BR15" s="8"/>
+      <c r="BS15" s="8"/>
+      <c r="BT15" s="8"/>
+      <c r="BU15" s="8"/>
+      <c r="BV15" s="8"/>
+      <c r="BW15" s="8"/>
+      <c r="BX15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY15" s="8"/>
+      <c r="BZ15" s="8"/>
+      <c r="CA15" s="8"/>
+      <c r="CB15" s="8"/>
+      <c r="CC15" s="8"/>
+      <c r="CD15" s="8"/>
+      <c r="CE15" s="5"/>
+      <c r="CF15" s="5"/>
+      <c r="CG15" s="5"/>
+      <c r="CH15" s="5"/>
+      <c r="CI15" s="5"/>
+      <c r="CJ15" s="5"/>
+      <c r="CK15" s="5"/>
+      <c r="CL15" s="5"/>
+      <c r="CM15" s="5"/>
+      <c r="CN15" s="5"/>
+      <c r="CO15" s="5"/>
+      <c r="CP15" s="5"/>
+      <c r="CQ15" s="5"/>
+      <c r="CR15" s="5"/>
+      <c r="CS15" s="5"/>
+      <c r="CT15" s="5"/>
+      <c r="CU15" s="5"/>
+      <c r="CV15" s="5"/>
+      <c r="CW15" s="5"/>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1766,12 +2359,52 @@
       <c r="BI16" s="4"/>
       <c r="BJ16" s="4"/>
       <c r="BK16" s="4"/>
+      <c r="BL16" s="8"/>
+      <c r="BM16" s="8"/>
+      <c r="BN16" s="8"/>
+      <c r="BO16" s="8"/>
+      <c r="BP16" s="8"/>
+      <c r="BQ16" s="8"/>
+      <c r="BR16" s="8"/>
+      <c r="BS16" s="8"/>
+      <c r="BT16" s="8"/>
+      <c r="BU16" s="8"/>
+      <c r="BV16" s="8"/>
+      <c r="BW16" s="8"/>
+      <c r="BX16" s="8"/>
+      <c r="BY16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BZ16" s="8"/>
+      <c r="CA16" s="8"/>
+      <c r="CB16" s="8"/>
+      <c r="CC16" s="8"/>
+      <c r="CD16" s="8"/>
+      <c r="CE16" s="5"/>
+      <c r="CF16" s="5"/>
+      <c r="CG16" s="5"/>
+      <c r="CH16" s="5"/>
+      <c r="CI16" s="5"/>
+      <c r="CJ16" s="5"/>
+      <c r="CK16" s="5"/>
+      <c r="CL16" s="5"/>
+      <c r="CM16" s="5"/>
+      <c r="CN16" s="5"/>
+      <c r="CO16" s="5"/>
+      <c r="CP16" s="5"/>
+      <c r="CQ16" s="5"/>
+      <c r="CR16" s="5"/>
+      <c r="CS16" s="5"/>
+      <c r="CT16" s="5"/>
+      <c r="CU16" s="5"/>
+      <c r="CV16" s="5"/>
+      <c r="CW16" s="5"/>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1845,12 +2478,52 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
+      <c r="BL17" s="8"/>
+      <c r="BM17" s="8"/>
+      <c r="BN17" s="8"/>
+      <c r="BO17" s="8"/>
+      <c r="BP17" s="8"/>
+      <c r="BQ17" s="8"/>
+      <c r="BR17" s="8"/>
+      <c r="BS17" s="8"/>
+      <c r="BT17" s="8"/>
+      <c r="BU17" s="8"/>
+      <c r="BV17" s="8"/>
+      <c r="BW17" s="8"/>
+      <c r="BX17" s="8"/>
+      <c r="BY17" s="8"/>
+      <c r="BZ17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CA17" s="8"/>
+      <c r="CB17" s="8"/>
+      <c r="CC17" s="8"/>
+      <c r="CD17" s="8"/>
+      <c r="CE17" s="5"/>
+      <c r="CF17" s="5"/>
+      <c r="CG17" s="5"/>
+      <c r="CH17" s="5"/>
+      <c r="CI17" s="5"/>
+      <c r="CJ17" s="5"/>
+      <c r="CK17" s="5"/>
+      <c r="CL17" s="5"/>
+      <c r="CM17" s="5"/>
+      <c r="CN17" s="5"/>
+      <c r="CO17" s="5"/>
+      <c r="CP17" s="5"/>
+      <c r="CQ17" s="5"/>
+      <c r="CR17" s="5"/>
+      <c r="CS17" s="5"/>
+      <c r="CT17" s="5"/>
+      <c r="CU17" s="5"/>
+      <c r="CV17" s="5"/>
+      <c r="CW17" s="5"/>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1924,12 +2597,54 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
+      <c r="BL18" s="8"/>
+      <c r="BM18" s="8"/>
+      <c r="BN18" s="8"/>
+      <c r="BO18" s="8"/>
+      <c r="BP18" s="8"/>
+      <c r="BQ18" s="8"/>
+      <c r="BR18" s="8"/>
+      <c r="BS18" s="8"/>
+      <c r="BT18" s="8"/>
+      <c r="BU18" s="8"/>
+      <c r="BV18" s="8"/>
+      <c r="BW18" s="8"/>
+      <c r="BX18" s="8"/>
+      <c r="BY18" s="8"/>
+      <c r="BZ18" s="8"/>
+      <c r="CA18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CB18" s="8"/>
+      <c r="CC18" s="8"/>
+      <c r="CD18" s="8"/>
+      <c r="CE18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+      <c r="CJ18" s="5"/>
+      <c r="CK18" s="5"/>
+      <c r="CL18" s="5"/>
+      <c r="CM18" s="5"/>
+      <c r="CN18" s="5"/>
+      <c r="CO18" s="5"/>
+      <c r="CP18" s="5"/>
+      <c r="CQ18" s="5"/>
+      <c r="CR18" s="5"/>
+      <c r="CS18" s="5"/>
+      <c r="CT18" s="5"/>
+      <c r="CU18" s="5"/>
+      <c r="CV18" s="5"/>
+      <c r="CW18" s="5"/>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1995,12 +2710,52 @@
       <c r="BI19" s="4"/>
       <c r="BJ19" s="4"/>
       <c r="BK19" s="4"/>
+      <c r="BL19" s="8"/>
+      <c r="BM19" s="8"/>
+      <c r="BN19" s="8"/>
+      <c r="BO19" s="8"/>
+      <c r="BP19" s="8"/>
+      <c r="BQ19" s="8"/>
+      <c r="BR19" s="8"/>
+      <c r="BS19" s="8"/>
+      <c r="BT19" s="8"/>
+      <c r="BU19" s="8"/>
+      <c r="BV19" s="8"/>
+      <c r="BW19" s="8"/>
+      <c r="BX19" s="8"/>
+      <c r="BY19" s="8"/>
+      <c r="BZ19" s="8"/>
+      <c r="CA19" s="8"/>
+      <c r="CB19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CC19" s="8"/>
+      <c r="CD19" s="8"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+      <c r="CK19" s="5"/>
+      <c r="CL19" s="5"/>
+      <c r="CM19" s="5"/>
+      <c r="CN19" s="5"/>
+      <c r="CO19" s="5"/>
+      <c r="CP19" s="5"/>
+      <c r="CQ19" s="5"/>
+      <c r="CR19" s="5"/>
+      <c r="CS19" s="5"/>
+      <c r="CT19" s="5"/>
+      <c r="CU19" s="5"/>
+      <c r="CV19" s="5"/>
+      <c r="CW19" s="5"/>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2064,12 +2819,52 @@
       </c>
       <c r="BJ20" s="4"/>
       <c r="BK20" s="4"/>
+      <c r="BL20" s="8"/>
+      <c r="BM20" s="8"/>
+      <c r="BN20" s="8"/>
+      <c r="BO20" s="8"/>
+      <c r="BP20" s="8"/>
+      <c r="BQ20" s="8"/>
+      <c r="BR20" s="8"/>
+      <c r="BS20" s="8"/>
+      <c r="BT20" s="8"/>
+      <c r="BU20" s="8"/>
+      <c r="BV20" s="8"/>
+      <c r="BW20" s="8"/>
+      <c r="BX20" s="8"/>
+      <c r="BY20" s="8"/>
+      <c r="BZ20" s="8"/>
+      <c r="CA20" s="8"/>
+      <c r="CB20" s="8"/>
+      <c r="CC20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CD20" s="8"/>
+      <c r="CE20" s="5"/>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+      <c r="CJ20" s="5"/>
+      <c r="CK20" s="5"/>
+      <c r="CL20" s="5"/>
+      <c r="CM20" s="5"/>
+      <c r="CN20" s="5"/>
+      <c r="CO20" s="5"/>
+      <c r="CP20" s="5"/>
+      <c r="CQ20" s="5"/>
+      <c r="CR20" s="5"/>
+      <c r="CS20" s="5"/>
+      <c r="CT20" s="5"/>
+      <c r="CU20" s="5"/>
+      <c r="CV20" s="5"/>
+      <c r="CW20" s="5"/>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2135,9 +2930,62 @@
       <c r="BK21" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="BL21" s="8"/>
+      <c r="BM21" s="8"/>
+      <c r="BN21" s="8"/>
+      <c r="BO21" s="8"/>
+      <c r="BP21" s="8"/>
+      <c r="BQ21" s="8"/>
+      <c r="BR21" s="8"/>
+      <c r="BS21" s="8"/>
+      <c r="BT21" s="8"/>
+      <c r="BU21" s="8"/>
+      <c r="BV21" s="8"/>
+      <c r="BW21" s="8"/>
+      <c r="BX21" s="8"/>
+      <c r="BY21" s="8"/>
+      <c r="BZ21" s="8"/>
+      <c r="CA21" s="8"/>
+      <c r="CB21" s="8"/>
+      <c r="CC21" s="8"/>
+      <c r="CD21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="CE21" s="5"/>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+      <c r="CJ21" s="5"/>
+      <c r="CK21" s="5"/>
+      <c r="CL21" s="5"/>
+      <c r="CM21" s="5"/>
+      <c r="CN21" s="5"/>
+      <c r="CO21" s="5"/>
+      <c r="CP21" s="5"/>
+      <c r="CQ21" s="5"/>
+      <c r="CR21" s="5"/>
+      <c r="CS21" s="5"/>
+      <c r="CT21" s="5"/>
+      <c r="CU21" s="5"/>
+      <c r="CV21" s="5"/>
+      <c r="CW21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
+    <mergeCell ref="BL2:CD2"/>
+    <mergeCell ref="CE2:CW2"/>
+    <mergeCell ref="AQ2:BK2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="AF2:AP2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="V2:AA2"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -2154,17 +3002,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AQ2:BK2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="AF2:AP2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="V2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into Codice"
This reverts commit bb703173abc4fc1ec10fc5988399e3fa87ef8efa, reversing
changes made to 29a4ede5827a60342091529ba90b93090490a0c7.
</commit_message>
<xml_diff>
--- a/NC09_Matrice_di_tracciabilità.xlsx
+++ b/NC09_Matrice_di_tracciabilità.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B8F4D4-36BF-4693-BD41-3C72A33A6934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Requisiti</t>
   </si>
@@ -230,42 +229,12 @@
   </si>
   <si>
     <t>Inventario</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Implementato</t>
-  </si>
-  <si>
-    <t>Sì</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Test Case</t>
-  </si>
-  <si>
-    <t>TC_C_1</t>
-  </si>
-  <si>
-    <t>TC_I_1</t>
-  </si>
-  <si>
-    <t>TC_A_1</t>
-  </si>
-  <si>
-    <t>TC_I_2</t>
-  </si>
-  <si>
-    <t>TC_U_1</t>
-  </si>
-  <si>
-    <t>TC_C_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -378,7 +347,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
@@ -393,9 +362,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -406,10 +372,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -694,16 +660,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CW21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BU1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CN6" sqref="CN6"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AR4" sqref="AR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -712,28 +678,28 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
       <c r="P2" s="13" t="s">
         <v>35</v>
       </c>
@@ -769,77 +735,35 @@
       <c r="AN2" s="13"/>
       <c r="AO2" s="13"/>
       <c r="AP2" s="13"/>
-      <c r="AQ2" s="9" t="s">
+      <c r="AQ2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="10"/>
-      <c r="AY2" s="10"/>
-      <c r="AZ2" s="10"/>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="10"/>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="10"/>
-      <c r="BE2" s="10"/>
-      <c r="BF2" s="10"/>
-      <c r="BG2" s="10"/>
-      <c r="BH2" s="10"/>
-      <c r="BI2" s="10"/>
-      <c r="BJ2" s="10"/>
-      <c r="BK2" s="11"/>
-      <c r="BL2" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM2" s="10"/>
-      <c r="BN2" s="10"/>
-      <c r="BO2" s="10"/>
-      <c r="BP2" s="10"/>
-      <c r="BQ2" s="10"/>
-      <c r="BR2" s="10"/>
-      <c r="BS2" s="10"/>
-      <c r="BT2" s="10"/>
-      <c r="BU2" s="10"/>
-      <c r="BV2" s="10"/>
-      <c r="BW2" s="10"/>
-      <c r="BX2" s="10"/>
-      <c r="BY2" s="10"/>
-      <c r="BZ2" s="10"/>
-      <c r="CA2" s="10"/>
-      <c r="CB2" s="10"/>
-      <c r="CC2" s="10"/>
-      <c r="CD2" s="10"/>
-      <c r="CE2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="CF2" s="10"/>
-      <c r="CG2" s="10"/>
-      <c r="CH2" s="10"/>
-      <c r="CI2" s="10"/>
-      <c r="CJ2" s="10"/>
-      <c r="CK2" s="10"/>
-      <c r="CL2" s="10"/>
-      <c r="CM2" s="10"/>
-      <c r="CN2" s="10"/>
-      <c r="CO2" s="10"/>
-      <c r="CP2" s="10"/>
-      <c r="CQ2" s="10"/>
-      <c r="CR2" s="10"/>
-      <c r="CS2" s="10"/>
-      <c r="CT2" s="10"/>
-      <c r="CU2" s="10"/>
-      <c r="CV2" s="10"/>
-      <c r="CW2" s="10"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="AZ2" s="9"/>
+      <c r="BA2" s="9"/>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BJ2" s="9"/>
+      <c r="BK2" s="10"/>
     </row>
-    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -905,54 +829,12 @@
       <c r="BI3" s="4"/>
       <c r="BJ3" s="4"/>
       <c r="BK3" s="4"/>
-      <c r="BL3" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="8"/>
-      <c r="BR3" s="8"/>
-      <c r="BS3" s="8"/>
-      <c r="BT3" s="8"/>
-      <c r="BU3" s="8"/>
-      <c r="BV3" s="8"/>
-      <c r="BW3" s="8"/>
-      <c r="BX3" s="8"/>
-      <c r="BY3" s="8"/>
-      <c r="BZ3" s="8"/>
-      <c r="CA3" s="8"/>
-      <c r="CB3" s="8"/>
-      <c r="CC3" s="8"/>
-      <c r="CD3" s="8"/>
-      <c r="CE3" s="5"/>
-      <c r="CF3" s="5"/>
-      <c r="CG3" s="5"/>
-      <c r="CH3" s="5"/>
-      <c r="CI3" s="5"/>
-      <c r="CJ3" s="5"/>
-      <c r="CK3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CL3" s="5"/>
-      <c r="CM3" s="5"/>
-      <c r="CN3" s="5"/>
-      <c r="CO3" s="5"/>
-      <c r="CP3" s="5"/>
-      <c r="CQ3" s="5"/>
-      <c r="CR3" s="5"/>
-      <c r="CS3" s="5"/>
-      <c r="CT3" s="5"/>
-      <c r="CU3" s="5"/>
-      <c r="CV3" s="5"/>
-      <c r="CW3" s="5"/>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1014,52 +896,12 @@
       <c r="BI4" s="4"/>
       <c r="BJ4" s="4"/>
       <c r="BK4" s="4"/>
-      <c r="BL4" s="8"/>
-      <c r="BM4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BN4" s="8"/>
-      <c r="BO4" s="8"/>
-      <c r="BP4" s="8"/>
-      <c r="BQ4" s="8"/>
-      <c r="BR4" s="8"/>
-      <c r="BS4" s="8"/>
-      <c r="BT4" s="8"/>
-      <c r="BU4" s="8"/>
-      <c r="BV4" s="8"/>
-      <c r="BW4" s="8"/>
-      <c r="BX4" s="8"/>
-      <c r="BY4" s="8"/>
-      <c r="BZ4" s="8"/>
-      <c r="CA4" s="8"/>
-      <c r="CB4" s="8"/>
-      <c r="CC4" s="8"/>
-      <c r="CD4" s="8"/>
-      <c r="CE4" s="5"/>
-      <c r="CF4" s="5"/>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-      <c r="CJ4" s="5"/>
-      <c r="CK4" s="5"/>
-      <c r="CL4" s="5"/>
-      <c r="CM4" s="5"/>
-      <c r="CN4" s="5"/>
-      <c r="CO4" s="5"/>
-      <c r="CP4" s="5"/>
-      <c r="CQ4" s="5"/>
-      <c r="CR4" s="5"/>
-      <c r="CS4" s="5"/>
-      <c r="CT4" s="5"/>
-      <c r="CU4" s="5"/>
-      <c r="CV4" s="5"/>
-      <c r="CW4" s="5"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1135,54 +977,12 @@
       <c r="BI5" s="4"/>
       <c r="BJ5" s="4"/>
       <c r="BK5" s="4"/>
-      <c r="BL5" s="8"/>
-      <c r="BM5" s="8"/>
-      <c r="BN5" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO5" s="8"/>
-      <c r="BP5" s="8"/>
-      <c r="BQ5" s="8"/>
-      <c r="BR5" s="8"/>
-      <c r="BS5" s="8"/>
-      <c r="BT5" s="8"/>
-      <c r="BU5" s="8"/>
-      <c r="BV5" s="8"/>
-      <c r="BW5" s="8"/>
-      <c r="BX5" s="8"/>
-      <c r="BY5" s="8"/>
-      <c r="BZ5" s="8"/>
-      <c r="CA5" s="8"/>
-      <c r="CB5" s="8"/>
-      <c r="CC5" s="8"/>
-      <c r="CD5" s="8"/>
-      <c r="CE5" s="5"/>
-      <c r="CF5" s="5"/>
-      <c r="CG5" s="5"/>
-      <c r="CH5" s="5"/>
-      <c r="CI5" s="5"/>
-      <c r="CJ5" s="5"/>
-      <c r="CK5" s="5"/>
-      <c r="CL5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CM5" s="5"/>
-      <c r="CN5" s="5"/>
-      <c r="CO5" s="5"/>
-      <c r="CP5" s="5"/>
-      <c r="CQ5" s="5"/>
-      <c r="CR5" s="5"/>
-      <c r="CS5" s="5"/>
-      <c r="CT5" s="5"/>
-      <c r="CU5" s="5"/>
-      <c r="CV5" s="5"/>
-      <c r="CW5" s="5"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1246,52 +1046,12 @@
       <c r="BI6" s="4"/>
       <c r="BJ6" s="4"/>
       <c r="BK6" s="4"/>
-      <c r="BL6" s="8"/>
-      <c r="BM6" s="8"/>
-      <c r="BN6" s="8"/>
-      <c r="BO6" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BP6" s="8"/>
-      <c r="BQ6" s="8"/>
-      <c r="BR6" s="8"/>
-      <c r="BS6" s="8"/>
-      <c r="BT6" s="8"/>
-      <c r="BU6" s="8"/>
-      <c r="BV6" s="8"/>
-      <c r="BW6" s="8"/>
-      <c r="BX6" s="8"/>
-      <c r="BY6" s="8"/>
-      <c r="BZ6" s="8"/>
-      <c r="CA6" s="8"/>
-      <c r="CB6" s="8"/>
-      <c r="CC6" s="8"/>
-      <c r="CD6" s="8"/>
-      <c r="CE6" s="5"/>
-      <c r="CF6" s="5"/>
-      <c r="CG6" s="5"/>
-      <c r="CH6" s="5"/>
-      <c r="CI6" s="5"/>
-      <c r="CJ6" s="5"/>
-      <c r="CK6" s="5"/>
-      <c r="CL6" s="5"/>
-      <c r="CM6" s="5"/>
-      <c r="CN6" s="5"/>
-      <c r="CO6" s="5"/>
-      <c r="CP6" s="5"/>
-      <c r="CQ6" s="5"/>
-      <c r="CR6" s="5"/>
-      <c r="CS6" s="5"/>
-      <c r="CT6" s="5"/>
-      <c r="CU6" s="5"/>
-      <c r="CV6" s="5"/>
-      <c r="CW6" s="5"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1357,54 +1117,12 @@
       <c r="BI7" s="4"/>
       <c r="BJ7" s="4"/>
       <c r="BK7" s="4"/>
-      <c r="BL7" s="8"/>
-      <c r="BM7" s="8"/>
-      <c r="BN7" s="8"/>
-      <c r="BO7" s="8"/>
-      <c r="BP7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BQ7" s="8"/>
-      <c r="BR7" s="8"/>
-      <c r="BS7" s="8"/>
-      <c r="BT7" s="8"/>
-      <c r="BU7" s="8"/>
-      <c r="BV7" s="8"/>
-      <c r="BW7" s="8"/>
-      <c r="BX7" s="8"/>
-      <c r="BY7" s="8"/>
-      <c r="BZ7" s="8"/>
-      <c r="CA7" s="8"/>
-      <c r="CB7" s="8"/>
-      <c r="CC7" s="8"/>
-      <c r="CD7" s="8"/>
-      <c r="CE7" s="5"/>
-      <c r="CF7" s="5"/>
-      <c r="CG7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="CH7" s="5"/>
-      <c r="CI7" s="5"/>
-      <c r="CJ7" s="5"/>
-      <c r="CK7" s="5"/>
-      <c r="CL7" s="5"/>
-      <c r="CM7" s="5"/>
-      <c r="CN7" s="5"/>
-      <c r="CO7" s="5"/>
-      <c r="CP7" s="5"/>
-      <c r="CQ7" s="5"/>
-      <c r="CR7" s="5"/>
-      <c r="CS7" s="5"/>
-      <c r="CT7" s="5"/>
-      <c r="CU7" s="5"/>
-      <c r="CV7" s="5"/>
-      <c r="CW7" s="5"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1468,54 +1186,12 @@
       <c r="BI8" s="4"/>
       <c r="BJ8" s="4"/>
       <c r="BK8" s="4"/>
-      <c r="BL8" s="8"/>
-      <c r="BM8" s="8"/>
-      <c r="BN8" s="8"/>
-      <c r="BO8" s="8"/>
-      <c r="BP8" s="8"/>
-      <c r="BQ8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BR8" s="8"/>
-      <c r="BS8" s="8"/>
-      <c r="BT8" s="8"/>
-      <c r="BU8" s="8"/>
-      <c r="BV8" s="8"/>
-      <c r="BW8" s="8"/>
-      <c r="BX8" s="8"/>
-      <c r="BY8" s="8"/>
-      <c r="BZ8" s="8"/>
-      <c r="CA8" s="8"/>
-      <c r="CB8" s="8"/>
-      <c r="CC8" s="8"/>
-      <c r="CD8" s="8"/>
-      <c r="CE8" s="5"/>
-      <c r="CF8" s="5"/>
-      <c r="CG8" s="5"/>
-      <c r="CH8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI8" s="5"/>
-      <c r="CJ8" s="5"/>
-      <c r="CK8" s="5"/>
-      <c r="CL8" s="5"/>
-      <c r="CM8" s="5"/>
-      <c r="CN8" s="5"/>
-      <c r="CO8" s="5"/>
-      <c r="CP8" s="5"/>
-      <c r="CQ8" s="5"/>
-      <c r="CR8" s="5"/>
-      <c r="CS8" s="5"/>
-      <c r="CT8" s="5"/>
-      <c r="CU8" s="5"/>
-      <c r="CV8" s="5"/>
-      <c r="CW8" s="5"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1583,54 +1259,12 @@
       <c r="BI9" s="4"/>
       <c r="BJ9" s="4"/>
       <c r="BK9" s="4"/>
-      <c r="BL9" s="8"/>
-      <c r="BM9" s="8"/>
-      <c r="BN9" s="8"/>
-      <c r="BO9" s="8"/>
-      <c r="BP9" s="8"/>
-      <c r="BQ9" s="8"/>
-      <c r="BR9" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BS9" s="8"/>
-      <c r="BT9" s="8"/>
-      <c r="BU9" s="8"/>
-      <c r="BV9" s="8"/>
-      <c r="BW9" s="8"/>
-      <c r="BX9" s="8"/>
-      <c r="BY9" s="8"/>
-      <c r="BZ9" s="8"/>
-      <c r="CA9" s="8"/>
-      <c r="CB9" s="8"/>
-      <c r="CC9" s="8"/>
-      <c r="CD9" s="8"/>
-      <c r="CE9" s="5"/>
-      <c r="CF9" s="5"/>
-      <c r="CG9" s="5"/>
-      <c r="CH9" s="5"/>
-      <c r="CI9" s="5"/>
-      <c r="CJ9" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="CK9" s="5"/>
-      <c r="CL9" s="5"/>
-      <c r="CM9" s="5"/>
-      <c r="CN9" s="5"/>
-      <c r="CO9" s="5"/>
-      <c r="CP9" s="5"/>
-      <c r="CQ9" s="5"/>
-      <c r="CR9" s="5"/>
-      <c r="CS9" s="5"/>
-      <c r="CT9" s="5"/>
-      <c r="CU9" s="5"/>
-      <c r="CV9" s="5"/>
-      <c r="CW9" s="5"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1692,52 +1326,12 @@
       <c r="BI10" s="4"/>
       <c r="BJ10" s="4"/>
       <c r="BK10" s="4"/>
-      <c r="BL10" s="8"/>
-      <c r="BM10" s="8"/>
-      <c r="BN10" s="8"/>
-      <c r="BO10" s="8"/>
-      <c r="BP10" s="8"/>
-      <c r="BQ10" s="8"/>
-      <c r="BR10" s="8"/>
-      <c r="BS10" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BT10" s="8"/>
-      <c r="BU10" s="8"/>
-      <c r="BV10" s="8"/>
-      <c r="BW10" s="8"/>
-      <c r="BX10" s="8"/>
-      <c r="BY10" s="8"/>
-      <c r="BZ10" s="8"/>
-      <c r="CA10" s="8"/>
-      <c r="CB10" s="8"/>
-      <c r="CC10" s="8"/>
-      <c r="CD10" s="8"/>
-      <c r="CE10" s="5"/>
-      <c r="CF10" s="5"/>
-      <c r="CG10" s="5"/>
-      <c r="CH10" s="5"/>
-      <c r="CI10" s="5"/>
-      <c r="CJ10" s="5"/>
-      <c r="CK10" s="5"/>
-      <c r="CL10" s="5"/>
-      <c r="CM10" s="5"/>
-      <c r="CN10" s="5"/>
-      <c r="CO10" s="5"/>
-      <c r="CP10" s="5"/>
-      <c r="CQ10" s="5"/>
-      <c r="CR10" s="5"/>
-      <c r="CS10" s="5"/>
-      <c r="CT10" s="5"/>
-      <c r="CU10" s="5"/>
-      <c r="CV10" s="5"/>
-      <c r="CW10" s="5"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1799,52 +1393,12 @@
       <c r="BI11" s="4"/>
       <c r="BJ11" s="4"/>
       <c r="BK11" s="4"/>
-      <c r="BL11" s="8"/>
-      <c r="BM11" s="8"/>
-      <c r="BN11" s="8"/>
-      <c r="BO11" s="8"/>
-      <c r="BP11" s="8"/>
-      <c r="BQ11" s="8"/>
-      <c r="BR11" s="8"/>
-      <c r="BS11" s="8"/>
-      <c r="BT11" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BU11" s="8"/>
-      <c r="BV11" s="8"/>
-      <c r="BW11" s="8"/>
-      <c r="BX11" s="8"/>
-      <c r="BY11" s="8"/>
-      <c r="BZ11" s="8"/>
-      <c r="CA11" s="8"/>
-      <c r="CB11" s="8"/>
-      <c r="CC11" s="8"/>
-      <c r="CD11" s="8"/>
-      <c r="CE11" s="5"/>
-      <c r="CF11" s="5"/>
-      <c r="CG11" s="5"/>
-      <c r="CH11" s="5"/>
-      <c r="CI11" s="5"/>
-      <c r="CJ11" s="5"/>
-      <c r="CK11" s="5"/>
-      <c r="CL11" s="5"/>
-      <c r="CM11" s="5"/>
-      <c r="CN11" s="5"/>
-      <c r="CO11" s="5"/>
-      <c r="CP11" s="5"/>
-      <c r="CQ11" s="5"/>
-      <c r="CR11" s="5"/>
-      <c r="CS11" s="5"/>
-      <c r="CT11" s="5"/>
-      <c r="CU11" s="5"/>
-      <c r="CV11" s="5"/>
-      <c r="CW11" s="5"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1908,52 +1462,12 @@
       <c r="BI12" s="4"/>
       <c r="BJ12" s="4"/>
       <c r="BK12" s="4"/>
-      <c r="BL12" s="8"/>
-      <c r="BM12" s="8"/>
-      <c r="BN12" s="8"/>
-      <c r="BO12" s="8"/>
-      <c r="BP12" s="8"/>
-      <c r="BQ12" s="8"/>
-      <c r="BR12" s="8"/>
-      <c r="BS12" s="8"/>
-      <c r="BT12" s="8"/>
-      <c r="BU12" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BV12" s="8"/>
-      <c r="BW12" s="8"/>
-      <c r="BX12" s="8"/>
-      <c r="BY12" s="8"/>
-      <c r="BZ12" s="8"/>
-      <c r="CA12" s="8"/>
-      <c r="CB12" s="8"/>
-      <c r="CC12" s="8"/>
-      <c r="CD12" s="8"/>
-      <c r="CE12" s="5"/>
-      <c r="CF12" s="5"/>
-      <c r="CG12" s="5"/>
-      <c r="CH12" s="5"/>
-      <c r="CI12" s="5"/>
-      <c r="CJ12" s="5"/>
-      <c r="CK12" s="5"/>
-      <c r="CL12" s="5"/>
-      <c r="CM12" s="5"/>
-      <c r="CN12" s="5"/>
-      <c r="CO12" s="5"/>
-      <c r="CP12" s="5"/>
-      <c r="CQ12" s="5"/>
-      <c r="CR12" s="5"/>
-      <c r="CS12" s="5"/>
-      <c r="CT12" s="5"/>
-      <c r="CU12" s="5"/>
-      <c r="CV12" s="5"/>
-      <c r="CW12" s="5"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
@@ -2027,54 +1541,12 @@
       <c r="BI13" s="4"/>
       <c r="BJ13" s="4"/>
       <c r="BK13" s="4"/>
-      <c r="BL13" s="8"/>
-      <c r="BM13" s="8"/>
-      <c r="BN13" s="8"/>
-      <c r="BO13" s="8"/>
-      <c r="BP13" s="8"/>
-      <c r="BQ13" s="8"/>
-      <c r="BR13" s="8"/>
-      <c r="BS13" s="8"/>
-      <c r="BT13" s="8"/>
-      <c r="BU13" s="8"/>
-      <c r="BV13" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BW13" s="8"/>
-      <c r="BX13" s="8"/>
-      <c r="BY13" s="8"/>
-      <c r="BZ13" s="8"/>
-      <c r="CA13" s="8"/>
-      <c r="CB13" s="8"/>
-      <c r="CC13" s="8"/>
-      <c r="CD13" s="8"/>
-      <c r="CE13" s="5"/>
-      <c r="CF13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="CG13" s="5"/>
-      <c r="CH13" s="5"/>
-      <c r="CI13" s="5"/>
-      <c r="CJ13" s="5"/>
-      <c r="CK13" s="5"/>
-      <c r="CL13" s="5"/>
-      <c r="CM13" s="5"/>
-      <c r="CN13" s="5"/>
-      <c r="CO13" s="5"/>
-      <c r="CP13" s="5"/>
-      <c r="CQ13" s="5"/>
-      <c r="CR13" s="5"/>
-      <c r="CS13" s="5"/>
-      <c r="CT13" s="5"/>
-      <c r="CU13" s="5"/>
-      <c r="CV13" s="5"/>
-      <c r="CW13" s="5"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -2148,54 +1620,12 @@
       <c r="BI14" s="4"/>
       <c r="BJ14" s="4"/>
       <c r="BK14" s="4"/>
-      <c r="BL14" s="8"/>
-      <c r="BM14" s="8"/>
-      <c r="BN14" s="8"/>
-      <c r="BO14" s="8"/>
-      <c r="BP14" s="8"/>
-      <c r="BQ14" s="8"/>
-      <c r="BR14" s="8"/>
-      <c r="BS14" s="8"/>
-      <c r="BT14" s="8"/>
-      <c r="BU14" s="8"/>
-      <c r="BV14" s="8"/>
-      <c r="BW14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BX14" s="8"/>
-      <c r="BY14" s="8"/>
-      <c r="BZ14" s="8"/>
-      <c r="CA14" s="8"/>
-      <c r="CB14" s="8"/>
-      <c r="CC14" s="8"/>
-      <c r="CD14" s="8"/>
-      <c r="CE14" s="5"/>
-      <c r="CF14" s="5"/>
-      <c r="CG14" s="5"/>
-      <c r="CH14" s="5"/>
-      <c r="CI14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="CJ14" s="5"/>
-      <c r="CK14" s="5"/>
-      <c r="CL14" s="5"/>
-      <c r="CM14" s="5"/>
-      <c r="CN14" s="5"/>
-      <c r="CO14" s="5"/>
-      <c r="CP14" s="5"/>
-      <c r="CQ14" s="5"/>
-      <c r="CR14" s="5"/>
-      <c r="CS14" s="5"/>
-      <c r="CT14" s="5"/>
-      <c r="CU14" s="5"/>
-      <c r="CV14" s="5"/>
-      <c r="CW14" s="5"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -2257,52 +1687,12 @@
       <c r="BI15" s="4"/>
       <c r="BJ15" s="4"/>
       <c r="BK15" s="4"/>
-      <c r="BL15" s="8"/>
-      <c r="BM15" s="8"/>
-      <c r="BN15" s="8"/>
-      <c r="BO15" s="8"/>
-      <c r="BP15" s="8"/>
-      <c r="BQ15" s="8"/>
-      <c r="BR15" s="8"/>
-      <c r="BS15" s="8"/>
-      <c r="BT15" s="8"/>
-      <c r="BU15" s="8"/>
-      <c r="BV15" s="8"/>
-      <c r="BW15" s="8"/>
-      <c r="BX15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="BY15" s="8"/>
-      <c r="BZ15" s="8"/>
-      <c r="CA15" s="8"/>
-      <c r="CB15" s="8"/>
-      <c r="CC15" s="8"/>
-      <c r="CD15" s="8"/>
-      <c r="CE15" s="5"/>
-      <c r="CF15" s="5"/>
-      <c r="CG15" s="5"/>
-      <c r="CH15" s="5"/>
-      <c r="CI15" s="5"/>
-      <c r="CJ15" s="5"/>
-      <c r="CK15" s="5"/>
-      <c r="CL15" s="5"/>
-      <c r="CM15" s="5"/>
-      <c r="CN15" s="5"/>
-      <c r="CO15" s="5"/>
-      <c r="CP15" s="5"/>
-      <c r="CQ15" s="5"/>
-      <c r="CR15" s="5"/>
-      <c r="CS15" s="5"/>
-      <c r="CT15" s="5"/>
-      <c r="CU15" s="5"/>
-      <c r="CV15" s="5"/>
-      <c r="CW15" s="5"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2376,52 +1766,12 @@
       <c r="BI16" s="4"/>
       <c r="BJ16" s="4"/>
       <c r="BK16" s="4"/>
-      <c r="BL16" s="8"/>
-      <c r="BM16" s="8"/>
-      <c r="BN16" s="8"/>
-      <c r="BO16" s="8"/>
-      <c r="BP16" s="8"/>
-      <c r="BQ16" s="8"/>
-      <c r="BR16" s="8"/>
-      <c r="BS16" s="8"/>
-      <c r="BT16" s="8"/>
-      <c r="BU16" s="8"/>
-      <c r="BV16" s="8"/>
-      <c r="BW16" s="8"/>
-      <c r="BX16" s="8"/>
-      <c r="BY16" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="BZ16" s="8"/>
-      <c r="CA16" s="8"/>
-      <c r="CB16" s="8"/>
-      <c r="CC16" s="8"/>
-      <c r="CD16" s="8"/>
-      <c r="CE16" s="5"/>
-      <c r="CF16" s="5"/>
-      <c r="CG16" s="5"/>
-      <c r="CH16" s="5"/>
-      <c r="CI16" s="5"/>
-      <c r="CJ16" s="5"/>
-      <c r="CK16" s="5"/>
-      <c r="CL16" s="5"/>
-      <c r="CM16" s="5"/>
-      <c r="CN16" s="5"/>
-      <c r="CO16" s="5"/>
-      <c r="CP16" s="5"/>
-      <c r="CQ16" s="5"/>
-      <c r="CR16" s="5"/>
-      <c r="CS16" s="5"/>
-      <c r="CT16" s="5"/>
-      <c r="CU16" s="5"/>
-      <c r="CV16" s="5"/>
-      <c r="CW16" s="5"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -2495,52 +1845,12 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
-      <c r="BL17" s="8"/>
-      <c r="BM17" s="8"/>
-      <c r="BN17" s="8"/>
-      <c r="BO17" s="8"/>
-      <c r="BP17" s="8"/>
-      <c r="BQ17" s="8"/>
-      <c r="BR17" s="8"/>
-      <c r="BS17" s="8"/>
-      <c r="BT17" s="8"/>
-      <c r="BU17" s="8"/>
-      <c r="BV17" s="8"/>
-      <c r="BW17" s="8"/>
-      <c r="BX17" s="8"/>
-      <c r="BY17" s="8"/>
-      <c r="BZ17" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA17" s="8"/>
-      <c r="CB17" s="8"/>
-      <c r="CC17" s="8"/>
-      <c r="CD17" s="8"/>
-      <c r="CE17" s="5"/>
-      <c r="CF17" s="5"/>
-      <c r="CG17" s="5"/>
-      <c r="CH17" s="5"/>
-      <c r="CI17" s="5"/>
-      <c r="CJ17" s="5"/>
-      <c r="CK17" s="5"/>
-      <c r="CL17" s="5"/>
-      <c r="CM17" s="5"/>
-      <c r="CN17" s="5"/>
-      <c r="CO17" s="5"/>
-      <c r="CP17" s="5"/>
-      <c r="CQ17" s="5"/>
-      <c r="CR17" s="5"/>
-      <c r="CS17" s="5"/>
-      <c r="CT17" s="5"/>
-      <c r="CU17" s="5"/>
-      <c r="CV17" s="5"/>
-      <c r="CW17" s="5"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -2614,54 +1924,12 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
-      <c r="BL18" s="8"/>
-      <c r="BM18" s="8"/>
-      <c r="BN18" s="8"/>
-      <c r="BO18" s="8"/>
-      <c r="BP18" s="8"/>
-      <c r="BQ18" s="8"/>
-      <c r="BR18" s="8"/>
-      <c r="BS18" s="8"/>
-      <c r="BT18" s="8"/>
-      <c r="BU18" s="8"/>
-      <c r="BV18" s="8"/>
-      <c r="BW18" s="8"/>
-      <c r="BX18" s="8"/>
-      <c r="BY18" s="8"/>
-      <c r="BZ18" s="8"/>
-      <c r="CA18" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB18" s="8"/>
-      <c r="CC18" s="8"/>
-      <c r="CD18" s="8"/>
-      <c r="CE18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="CF18" s="5"/>
-      <c r="CG18" s="5"/>
-      <c r="CH18" s="5"/>
-      <c r="CI18" s="5"/>
-      <c r="CJ18" s="5"/>
-      <c r="CK18" s="5"/>
-      <c r="CL18" s="5"/>
-      <c r="CM18" s="5"/>
-      <c r="CN18" s="5"/>
-      <c r="CO18" s="5"/>
-      <c r="CP18" s="5"/>
-      <c r="CQ18" s="5"/>
-      <c r="CR18" s="5"/>
-      <c r="CS18" s="5"/>
-      <c r="CT18" s="5"/>
-      <c r="CU18" s="5"/>
-      <c r="CV18" s="5"/>
-      <c r="CW18" s="5"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -2727,52 +1995,12 @@
       <c r="BI19" s="4"/>
       <c r="BJ19" s="4"/>
       <c r="BK19" s="4"/>
-      <c r="BL19" s="8"/>
-      <c r="BM19" s="8"/>
-      <c r="BN19" s="8"/>
-      <c r="BO19" s="8"/>
-      <c r="BP19" s="8"/>
-      <c r="BQ19" s="8"/>
-      <c r="BR19" s="8"/>
-      <c r="BS19" s="8"/>
-      <c r="BT19" s="8"/>
-      <c r="BU19" s="8"/>
-      <c r="BV19" s="8"/>
-      <c r="BW19" s="8"/>
-      <c r="BX19" s="8"/>
-      <c r="BY19" s="8"/>
-      <c r="BZ19" s="8"/>
-      <c r="CA19" s="8"/>
-      <c r="CB19" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="CC19" s="8"/>
-      <c r="CD19" s="8"/>
-      <c r="CE19" s="5"/>
-      <c r="CF19" s="5"/>
-      <c r="CG19" s="5"/>
-      <c r="CH19" s="5"/>
-      <c r="CI19" s="5"/>
-      <c r="CJ19" s="5"/>
-      <c r="CK19" s="5"/>
-      <c r="CL19" s="5"/>
-      <c r="CM19" s="5"/>
-      <c r="CN19" s="5"/>
-      <c r="CO19" s="5"/>
-      <c r="CP19" s="5"/>
-      <c r="CQ19" s="5"/>
-      <c r="CR19" s="5"/>
-      <c r="CS19" s="5"/>
-      <c r="CT19" s="5"/>
-      <c r="CU19" s="5"/>
-      <c r="CV19" s="5"/>
-      <c r="CW19" s="5"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2836,52 +2064,12 @@
       </c>
       <c r="BJ20" s="4"/>
       <c r="BK20" s="4"/>
-      <c r="BL20" s="8"/>
-      <c r="BM20" s="8"/>
-      <c r="BN20" s="8"/>
-      <c r="BO20" s="8"/>
-      <c r="BP20" s="8"/>
-      <c r="BQ20" s="8"/>
-      <c r="BR20" s="8"/>
-      <c r="BS20" s="8"/>
-      <c r="BT20" s="8"/>
-      <c r="BU20" s="8"/>
-      <c r="BV20" s="8"/>
-      <c r="BW20" s="8"/>
-      <c r="BX20" s="8"/>
-      <c r="BY20" s="8"/>
-      <c r="BZ20" s="8"/>
-      <c r="CA20" s="8"/>
-      <c r="CB20" s="8"/>
-      <c r="CC20" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="CD20" s="8"/>
-      <c r="CE20" s="5"/>
-      <c r="CF20" s="5"/>
-      <c r="CG20" s="5"/>
-      <c r="CH20" s="5"/>
-      <c r="CI20" s="5"/>
-      <c r="CJ20" s="5"/>
-      <c r="CK20" s="5"/>
-      <c r="CL20" s="5"/>
-      <c r="CM20" s="5"/>
-      <c r="CN20" s="5"/>
-      <c r="CO20" s="5"/>
-      <c r="CP20" s="5"/>
-      <c r="CQ20" s="5"/>
-      <c r="CR20" s="5"/>
-      <c r="CS20" s="5"/>
-      <c r="CT20" s="5"/>
-      <c r="CU20" s="5"/>
-      <c r="CV20" s="5"/>
-      <c r="CW20" s="5"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2947,51 +2135,9 @@
       <c r="BK21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BL21" s="8"/>
-      <c r="BM21" s="8"/>
-      <c r="BN21" s="8"/>
-      <c r="BO21" s="8"/>
-      <c r="BP21" s="8"/>
-      <c r="BQ21" s="8"/>
-      <c r="BR21" s="8"/>
-      <c r="BS21" s="8"/>
-      <c r="BT21" s="8"/>
-      <c r="BU21" s="8"/>
-      <c r="BV21" s="8"/>
-      <c r="BW21" s="8"/>
-      <c r="BX21" s="8"/>
-      <c r="BY21" s="8"/>
-      <c r="BZ21" s="8"/>
-      <c r="CA21" s="8"/>
-      <c r="CB21" s="8"/>
-      <c r="CC21" s="8"/>
-      <c r="CD21" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="CE21" s="5"/>
-      <c r="CF21" s="5"/>
-      <c r="CG21" s="5"/>
-      <c r="CH21" s="5"/>
-      <c r="CI21" s="5"/>
-      <c r="CJ21" s="5"/>
-      <c r="CK21" s="5"/>
-      <c r="CL21" s="5"/>
-      <c r="CM21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="CN21" s="5"/>
-      <c r="CO21" s="5"/>
-      <c r="CP21" s="5"/>
-      <c r="CQ21" s="5"/>
-      <c r="CR21" s="5"/>
-      <c r="CS21" s="5"/>
-      <c r="CT21" s="5"/>
-      <c r="CU21" s="5"/>
-      <c r="CV21" s="5"/>
-      <c r="CW21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
+  <mergeCells count="27">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3008,6 +2154,9 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="AQ2:BK2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -3016,11 +2165,6 @@
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:AA2"/>
-    <mergeCell ref="BL2:CD2"/>
-    <mergeCell ref="CE2:CW2"/>
-    <mergeCell ref="AQ2:BK2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'Codice' into main"
This reverts commit 010f6ccc9c51589ec5bc72c148a3b6c869d1285a, reversing
changes made to eb2a817f6fed82a5a10890aad913fed045c555c5.
</commit_message>
<xml_diff>
--- a/NC09_Matrice_di_tracciabilità.xlsx
+++ b/NC09_Matrice_di_tracciabilità.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B8F4D4-36BF-4693-BD41-3C72A33A6934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>Requisiti</t>
   </si>
@@ -229,12 +230,42 @@
   </si>
   <si>
     <t>Inventario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementato</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>TC_C_1</t>
+  </si>
+  <si>
+    <t>TC_I_1</t>
+  </si>
+  <si>
+    <t>TC_A_1</t>
+  </si>
+  <si>
+    <t>TC_I_2</t>
+  </si>
+  <si>
+    <t>TC_U_1</t>
+  </si>
+  <si>
+    <t>TC_C_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -347,7 +378,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
@@ -362,6 +393,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,10 +406,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -660,16 +694,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CN6" sqref="CN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -678,28 +712,28 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
       <c r="P2" s="13" t="s">
         <v>35</v>
       </c>
@@ -735,35 +769,77 @@
       <c r="AN2" s="13"/>
       <c r="AO2" s="13"/>
       <c r="AP2" s="13"/>
-      <c r="AQ2" s="8" t="s">
+      <c r="AQ2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="10"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="10"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="10"/>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="10"/>
+      <c r="BV2" s="10"/>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="CF2" s="10"/>
+      <c r="CG2" s="10"/>
+      <c r="CH2" s="10"/>
+      <c r="CI2" s="10"/>
+      <c r="CJ2" s="10"/>
+      <c r="CK2" s="10"/>
+      <c r="CL2" s="10"/>
+      <c r="CM2" s="10"/>
+      <c r="CN2" s="10"/>
+      <c r="CO2" s="10"/>
+      <c r="CP2" s="10"/>
+      <c r="CQ2" s="10"/>
+      <c r="CR2" s="10"/>
+      <c r="CS2" s="10"/>
+      <c r="CT2" s="10"/>
+      <c r="CU2" s="10"/>
+      <c r="CV2" s="10"/>
+      <c r="CW2" s="10"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -829,12 +905,54 @@
       <c r="BI3" s="4"/>
       <c r="BJ3" s="4"/>
       <c r="BK3" s="4"/>
+      <c r="BL3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CE3" s="5"/>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="5"/>
+      <c r="CH3" s="5"/>
+      <c r="CI3" s="5"/>
+      <c r="CJ3" s="5"/>
+      <c r="CK3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL3" s="5"/>
+      <c r="CM3" s="5"/>
+      <c r="CN3" s="5"/>
+      <c r="CO3" s="5"/>
+      <c r="CP3" s="5"/>
+      <c r="CQ3" s="5"/>
+      <c r="CR3" s="5"/>
+      <c r="CS3" s="5"/>
+      <c r="CT3" s="5"/>
+      <c r="CU3" s="5"/>
+      <c r="CV3" s="5"/>
+      <c r="CW3" s="5"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -896,12 +1014,52 @@
       <c r="BI4" s="4"/>
       <c r="BJ4" s="4"/>
       <c r="BK4" s="4"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="8"/>
+      <c r="BR4" s="8"/>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="8"/>
+      <c r="BY4" s="8"/>
+      <c r="BZ4" s="8"/>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+      <c r="CK4" s="5"/>
+      <c r="CL4" s="5"/>
+      <c r="CM4" s="5"/>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
@@ -977,12 +1135,54 @@
       <c r="BI5" s="4"/>
       <c r="BJ5" s="4"/>
       <c r="BK5" s="4"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO5" s="8"/>
+      <c r="BP5" s="8"/>
+      <c r="BQ5" s="8"/>
+      <c r="BR5" s="8"/>
+      <c r="BS5" s="8"/>
+      <c r="BT5" s="8"/>
+      <c r="BU5" s="8"/>
+      <c r="BV5" s="8"/>
+      <c r="BW5" s="8"/>
+      <c r="BX5" s="8"/>
+      <c r="BY5" s="8"/>
+      <c r="BZ5" s="8"/>
+      <c r="CA5" s="8"/>
+      <c r="CB5" s="8"/>
+      <c r="CC5" s="8"/>
+      <c r="CD5" s="8"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+      <c r="CK5" s="5"/>
+      <c r="CL5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM5" s="5"/>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1046,12 +1246,52 @@
       <c r="BI6" s="4"/>
       <c r="BJ6" s="4"/>
       <c r="BK6" s="4"/>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="8"/>
+      <c r="BN6" s="8"/>
+      <c r="BO6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP6" s="8"/>
+      <c r="BQ6" s="8"/>
+      <c r="BR6" s="8"/>
+      <c r="BS6" s="8"/>
+      <c r="BT6" s="8"/>
+      <c r="BU6" s="8"/>
+      <c r="BV6" s="8"/>
+      <c r="BW6" s="8"/>
+      <c r="BX6" s="8"/>
+      <c r="BY6" s="8"/>
+      <c r="BZ6" s="8"/>
+      <c r="CA6" s="8"/>
+      <c r="CB6" s="8"/>
+      <c r="CC6" s="8"/>
+      <c r="CD6" s="8"/>
+      <c r="CE6" s="5"/>
+      <c r="CF6" s="5"/>
+      <c r="CG6" s="5"/>
+      <c r="CH6" s="5"/>
+      <c r="CI6" s="5"/>
+      <c r="CJ6" s="5"/>
+      <c r="CK6" s="5"/>
+      <c r="CL6" s="5"/>
+      <c r="CM6" s="5"/>
+      <c r="CN6" s="5"/>
+      <c r="CO6" s="5"/>
+      <c r="CP6" s="5"/>
+      <c r="CQ6" s="5"/>
+      <c r="CR6" s="5"/>
+      <c r="CS6" s="5"/>
+      <c r="CT6" s="5"/>
+      <c r="CU6" s="5"/>
+      <c r="CV6" s="5"/>
+      <c r="CW6" s="5"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1117,12 +1357,54 @@
       <c r="BI7" s="4"/>
       <c r="BJ7" s="4"/>
       <c r="BK7" s="4"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ7" s="8"/>
+      <c r="BR7" s="8"/>
+      <c r="BS7" s="8"/>
+      <c r="BT7" s="8"/>
+      <c r="BU7" s="8"/>
+      <c r="BV7" s="8"/>
+      <c r="BW7" s="8"/>
+      <c r="BX7" s="8"/>
+      <c r="BY7" s="8"/>
+      <c r="BZ7" s="8"/>
+      <c r="CA7" s="8"/>
+      <c r="CB7" s="8"/>
+      <c r="CC7" s="8"/>
+      <c r="CD7" s="8"/>
+      <c r="CE7" s="5"/>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+      <c r="CJ7" s="5"/>
+      <c r="CK7" s="5"/>
+      <c r="CL7" s="5"/>
+      <c r="CM7" s="5"/>
+      <c r="CN7" s="5"/>
+      <c r="CO7" s="5"/>
+      <c r="CP7" s="5"/>
+      <c r="CQ7" s="5"/>
+      <c r="CR7" s="5"/>
+      <c r="CS7" s="5"/>
+      <c r="CT7" s="5"/>
+      <c r="CU7" s="5"/>
+      <c r="CV7" s="5"/>
+      <c r="CW7" s="5"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1186,12 +1468,54 @@
       <c r="BI8" s="4"/>
       <c r="BJ8" s="4"/>
       <c r="BK8" s="4"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+      <c r="BQ8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR8" s="8"/>
+      <c r="BS8" s="8"/>
+      <c r="BT8" s="8"/>
+      <c r="BU8" s="8"/>
+      <c r="BV8" s="8"/>
+      <c r="BW8" s="8"/>
+      <c r="BX8" s="8"/>
+      <c r="BY8" s="8"/>
+      <c r="BZ8" s="8"/>
+      <c r="CA8" s="8"/>
+      <c r="CB8" s="8"/>
+      <c r="CC8" s="8"/>
+      <c r="CD8" s="8"/>
+      <c r="CE8" s="5"/>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI8" s="5"/>
+      <c r="CJ8" s="5"/>
+      <c r="CK8" s="5"/>
+      <c r="CL8" s="5"/>
+      <c r="CM8" s="5"/>
+      <c r="CN8" s="5"/>
+      <c r="CO8" s="5"/>
+      <c r="CP8" s="5"/>
+      <c r="CQ8" s="5"/>
+      <c r="CR8" s="5"/>
+      <c r="CS8" s="5"/>
+      <c r="CT8" s="5"/>
+      <c r="CU8" s="5"/>
+      <c r="CV8" s="5"/>
+      <c r="CW8" s="5"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1259,12 +1583,54 @@
       <c r="BI9" s="4"/>
       <c r="BJ9" s="4"/>
       <c r="BK9" s="4"/>
+      <c r="BL9" s="8"/>
+      <c r="BM9" s="8"/>
+      <c r="BN9" s="8"/>
+      <c r="BO9" s="8"/>
+      <c r="BP9" s="8"/>
+      <c r="BQ9" s="8"/>
+      <c r="BR9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS9" s="8"/>
+      <c r="BT9" s="8"/>
+      <c r="BU9" s="8"/>
+      <c r="BV9" s="8"/>
+      <c r="BW9" s="8"/>
+      <c r="BX9" s="8"/>
+      <c r="BY9" s="8"/>
+      <c r="BZ9" s="8"/>
+      <c r="CA9" s="8"/>
+      <c r="CB9" s="8"/>
+      <c r="CC9" s="8"/>
+      <c r="CD9" s="8"/>
+      <c r="CE9" s="5"/>
+      <c r="CF9" s="5"/>
+      <c r="CG9" s="5"/>
+      <c r="CH9" s="5"/>
+      <c r="CI9" s="5"/>
+      <c r="CJ9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CK9" s="5"/>
+      <c r="CL9" s="5"/>
+      <c r="CM9" s="5"/>
+      <c r="CN9" s="5"/>
+      <c r="CO9" s="5"/>
+      <c r="CP9" s="5"/>
+      <c r="CQ9" s="5"/>
+      <c r="CR9" s="5"/>
+      <c r="CS9" s="5"/>
+      <c r="CT9" s="5"/>
+      <c r="CU9" s="5"/>
+      <c r="CV9" s="5"/>
+      <c r="CW9" s="5"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1326,12 +1692,52 @@
       <c r="BI10" s="4"/>
       <c r="BJ10" s="4"/>
       <c r="BK10" s="4"/>
+      <c r="BL10" s="8"/>
+      <c r="BM10" s="8"/>
+      <c r="BN10" s="8"/>
+      <c r="BO10" s="8"/>
+      <c r="BP10" s="8"/>
+      <c r="BQ10" s="8"/>
+      <c r="BR10" s="8"/>
+      <c r="BS10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BT10" s="8"/>
+      <c r="BU10" s="8"/>
+      <c r="BV10" s="8"/>
+      <c r="BW10" s="8"/>
+      <c r="BX10" s="8"/>
+      <c r="BY10" s="8"/>
+      <c r="BZ10" s="8"/>
+      <c r="CA10" s="8"/>
+      <c r="CB10" s="8"/>
+      <c r="CC10" s="8"/>
+      <c r="CD10" s="8"/>
+      <c r="CE10" s="5"/>
+      <c r="CF10" s="5"/>
+      <c r="CG10" s="5"/>
+      <c r="CH10" s="5"/>
+      <c r="CI10" s="5"/>
+      <c r="CJ10" s="5"/>
+      <c r="CK10" s="5"/>
+      <c r="CL10" s="5"/>
+      <c r="CM10" s="5"/>
+      <c r="CN10" s="5"/>
+      <c r="CO10" s="5"/>
+      <c r="CP10" s="5"/>
+      <c r="CQ10" s="5"/>
+      <c r="CR10" s="5"/>
+      <c r="CS10" s="5"/>
+      <c r="CT10" s="5"/>
+      <c r="CU10" s="5"/>
+      <c r="CV10" s="5"/>
+      <c r="CW10" s="5"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1393,12 +1799,52 @@
       <c r="BI11" s="4"/>
       <c r="BJ11" s="4"/>
       <c r="BK11" s="4"/>
+      <c r="BL11" s="8"/>
+      <c r="BM11" s="8"/>
+      <c r="BN11" s="8"/>
+      <c r="BO11" s="8"/>
+      <c r="BP11" s="8"/>
+      <c r="BQ11" s="8"/>
+      <c r="BR11" s="8"/>
+      <c r="BS11" s="8"/>
+      <c r="BT11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU11" s="8"/>
+      <c r="BV11" s="8"/>
+      <c r="BW11" s="8"/>
+      <c r="BX11" s="8"/>
+      <c r="BY11" s="8"/>
+      <c r="BZ11" s="8"/>
+      <c r="CA11" s="8"/>
+      <c r="CB11" s="8"/>
+      <c r="CC11" s="8"/>
+      <c r="CD11" s="8"/>
+      <c r="CE11" s="5"/>
+      <c r="CF11" s="5"/>
+      <c r="CG11" s="5"/>
+      <c r="CH11" s="5"/>
+      <c r="CI11" s="5"/>
+      <c r="CJ11" s="5"/>
+      <c r="CK11" s="5"/>
+      <c r="CL11" s="5"/>
+      <c r="CM11" s="5"/>
+      <c r="CN11" s="5"/>
+      <c r="CO11" s="5"/>
+      <c r="CP11" s="5"/>
+      <c r="CQ11" s="5"/>
+      <c r="CR11" s="5"/>
+      <c r="CS11" s="5"/>
+      <c r="CT11" s="5"/>
+      <c r="CU11" s="5"/>
+      <c r="CV11" s="5"/>
+      <c r="CW11" s="5"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1462,12 +1908,52 @@
       <c r="BI12" s="4"/>
       <c r="BJ12" s="4"/>
       <c r="BK12" s="4"/>
+      <c r="BL12" s="8"/>
+      <c r="BM12" s="8"/>
+      <c r="BN12" s="8"/>
+      <c r="BO12" s="8"/>
+      <c r="BP12" s="8"/>
+      <c r="BQ12" s="8"/>
+      <c r="BR12" s="8"/>
+      <c r="BS12" s="8"/>
+      <c r="BT12" s="8"/>
+      <c r="BU12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV12" s="8"/>
+      <c r="BW12" s="8"/>
+      <c r="BX12" s="8"/>
+      <c r="BY12" s="8"/>
+      <c r="BZ12" s="8"/>
+      <c r="CA12" s="8"/>
+      <c r="CB12" s="8"/>
+      <c r="CC12" s="8"/>
+      <c r="CD12" s="8"/>
+      <c r="CE12" s="5"/>
+      <c r="CF12" s="5"/>
+      <c r="CG12" s="5"/>
+      <c r="CH12" s="5"/>
+      <c r="CI12" s="5"/>
+      <c r="CJ12" s="5"/>
+      <c r="CK12" s="5"/>
+      <c r="CL12" s="5"/>
+      <c r="CM12" s="5"/>
+      <c r="CN12" s="5"/>
+      <c r="CO12" s="5"/>
+      <c r="CP12" s="5"/>
+      <c r="CQ12" s="5"/>
+      <c r="CR12" s="5"/>
+      <c r="CS12" s="5"/>
+      <c r="CT12" s="5"/>
+      <c r="CU12" s="5"/>
+      <c r="CV12" s="5"/>
+      <c r="CW12" s="5"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
@@ -1541,12 +2027,54 @@
       <c r="BI13" s="4"/>
       <c r="BJ13" s="4"/>
       <c r="BK13" s="4"/>
+      <c r="BL13" s="8"/>
+      <c r="BM13" s="8"/>
+      <c r="BN13" s="8"/>
+      <c r="BO13" s="8"/>
+      <c r="BP13" s="8"/>
+      <c r="BQ13" s="8"/>
+      <c r="BR13" s="8"/>
+      <c r="BS13" s="8"/>
+      <c r="BT13" s="8"/>
+      <c r="BU13" s="8"/>
+      <c r="BV13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW13" s="8"/>
+      <c r="BX13" s="8"/>
+      <c r="BY13" s="8"/>
+      <c r="BZ13" s="8"/>
+      <c r="CA13" s="8"/>
+      <c r="CB13" s="8"/>
+      <c r="CC13" s="8"/>
+      <c r="CD13" s="8"/>
+      <c r="CE13" s="5"/>
+      <c r="CF13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG13" s="5"/>
+      <c r="CH13" s="5"/>
+      <c r="CI13" s="5"/>
+      <c r="CJ13" s="5"/>
+      <c r="CK13" s="5"/>
+      <c r="CL13" s="5"/>
+      <c r="CM13" s="5"/>
+      <c r="CN13" s="5"/>
+      <c r="CO13" s="5"/>
+      <c r="CP13" s="5"/>
+      <c r="CQ13" s="5"/>
+      <c r="CR13" s="5"/>
+      <c r="CS13" s="5"/>
+      <c r="CT13" s="5"/>
+      <c r="CU13" s="5"/>
+      <c r="CV13" s="5"/>
+      <c r="CW13" s="5"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1620,12 +2148,54 @@
       <c r="BI14" s="4"/>
       <c r="BJ14" s="4"/>
       <c r="BK14" s="4"/>
+      <c r="BL14" s="8"/>
+      <c r="BM14" s="8"/>
+      <c r="BN14" s="8"/>
+      <c r="BO14" s="8"/>
+      <c r="BP14" s="8"/>
+      <c r="BQ14" s="8"/>
+      <c r="BR14" s="8"/>
+      <c r="BS14" s="8"/>
+      <c r="BT14" s="8"/>
+      <c r="BU14" s="8"/>
+      <c r="BV14" s="8"/>
+      <c r="BW14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BX14" s="8"/>
+      <c r="BY14" s="8"/>
+      <c r="BZ14" s="8"/>
+      <c r="CA14" s="8"/>
+      <c r="CB14" s="8"/>
+      <c r="CC14" s="8"/>
+      <c r="CD14" s="8"/>
+      <c r="CE14" s="5"/>
+      <c r="CF14" s="5"/>
+      <c r="CG14" s="5"/>
+      <c r="CH14" s="5"/>
+      <c r="CI14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CJ14" s="5"/>
+      <c r="CK14" s="5"/>
+      <c r="CL14" s="5"/>
+      <c r="CM14" s="5"/>
+      <c r="CN14" s="5"/>
+      <c r="CO14" s="5"/>
+      <c r="CP14" s="5"/>
+      <c r="CQ14" s="5"/>
+      <c r="CR14" s="5"/>
+      <c r="CS14" s="5"/>
+      <c r="CT14" s="5"/>
+      <c r="CU14" s="5"/>
+      <c r="CV14" s="5"/>
+      <c r="CW14" s="5"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1687,12 +2257,52 @@
       <c r="BI15" s="4"/>
       <c r="BJ15" s="4"/>
       <c r="BK15" s="4"/>
+      <c r="BL15" s="8"/>
+      <c r="BM15" s="8"/>
+      <c r="BN15" s="8"/>
+      <c r="BO15" s="8"/>
+      <c r="BP15" s="8"/>
+      <c r="BQ15" s="8"/>
+      <c r="BR15" s="8"/>
+      <c r="BS15" s="8"/>
+      <c r="BT15" s="8"/>
+      <c r="BU15" s="8"/>
+      <c r="BV15" s="8"/>
+      <c r="BW15" s="8"/>
+      <c r="BX15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY15" s="8"/>
+      <c r="BZ15" s="8"/>
+      <c r="CA15" s="8"/>
+      <c r="CB15" s="8"/>
+      <c r="CC15" s="8"/>
+      <c r="CD15" s="8"/>
+      <c r="CE15" s="5"/>
+      <c r="CF15" s="5"/>
+      <c r="CG15" s="5"/>
+      <c r="CH15" s="5"/>
+      <c r="CI15" s="5"/>
+      <c r="CJ15" s="5"/>
+      <c r="CK15" s="5"/>
+      <c r="CL15" s="5"/>
+      <c r="CM15" s="5"/>
+      <c r="CN15" s="5"/>
+      <c r="CO15" s="5"/>
+      <c r="CP15" s="5"/>
+      <c r="CQ15" s="5"/>
+      <c r="CR15" s="5"/>
+      <c r="CS15" s="5"/>
+      <c r="CT15" s="5"/>
+      <c r="CU15" s="5"/>
+      <c r="CV15" s="5"/>
+      <c r="CW15" s="5"/>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1766,12 +2376,52 @@
       <c r="BI16" s="4"/>
       <c r="BJ16" s="4"/>
       <c r="BK16" s="4"/>
+      <c r="BL16" s="8"/>
+      <c r="BM16" s="8"/>
+      <c r="BN16" s="8"/>
+      <c r="BO16" s="8"/>
+      <c r="BP16" s="8"/>
+      <c r="BQ16" s="8"/>
+      <c r="BR16" s="8"/>
+      <c r="BS16" s="8"/>
+      <c r="BT16" s="8"/>
+      <c r="BU16" s="8"/>
+      <c r="BV16" s="8"/>
+      <c r="BW16" s="8"/>
+      <c r="BX16" s="8"/>
+      <c r="BY16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BZ16" s="8"/>
+      <c r="CA16" s="8"/>
+      <c r="CB16" s="8"/>
+      <c r="CC16" s="8"/>
+      <c r="CD16" s="8"/>
+      <c r="CE16" s="5"/>
+      <c r="CF16" s="5"/>
+      <c r="CG16" s="5"/>
+      <c r="CH16" s="5"/>
+      <c r="CI16" s="5"/>
+      <c r="CJ16" s="5"/>
+      <c r="CK16" s="5"/>
+      <c r="CL16" s="5"/>
+      <c r="CM16" s="5"/>
+      <c r="CN16" s="5"/>
+      <c r="CO16" s="5"/>
+      <c r="CP16" s="5"/>
+      <c r="CQ16" s="5"/>
+      <c r="CR16" s="5"/>
+      <c r="CS16" s="5"/>
+      <c r="CT16" s="5"/>
+      <c r="CU16" s="5"/>
+      <c r="CV16" s="5"/>
+      <c r="CW16" s="5"/>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1845,12 +2495,52 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
+      <c r="BL17" s="8"/>
+      <c r="BM17" s="8"/>
+      <c r="BN17" s="8"/>
+      <c r="BO17" s="8"/>
+      <c r="BP17" s="8"/>
+      <c r="BQ17" s="8"/>
+      <c r="BR17" s="8"/>
+      <c r="BS17" s="8"/>
+      <c r="BT17" s="8"/>
+      <c r="BU17" s="8"/>
+      <c r="BV17" s="8"/>
+      <c r="BW17" s="8"/>
+      <c r="BX17" s="8"/>
+      <c r="BY17" s="8"/>
+      <c r="BZ17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CA17" s="8"/>
+      <c r="CB17" s="8"/>
+      <c r="CC17" s="8"/>
+      <c r="CD17" s="8"/>
+      <c r="CE17" s="5"/>
+      <c r="CF17" s="5"/>
+      <c r="CG17" s="5"/>
+      <c r="CH17" s="5"/>
+      <c r="CI17" s="5"/>
+      <c r="CJ17" s="5"/>
+      <c r="CK17" s="5"/>
+      <c r="CL17" s="5"/>
+      <c r="CM17" s="5"/>
+      <c r="CN17" s="5"/>
+      <c r="CO17" s="5"/>
+      <c r="CP17" s="5"/>
+      <c r="CQ17" s="5"/>
+      <c r="CR17" s="5"/>
+      <c r="CS17" s="5"/>
+      <c r="CT17" s="5"/>
+      <c r="CU17" s="5"/>
+      <c r="CV17" s="5"/>
+      <c r="CW17" s="5"/>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1924,12 +2614,54 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
+      <c r="BL18" s="8"/>
+      <c r="BM18" s="8"/>
+      <c r="BN18" s="8"/>
+      <c r="BO18" s="8"/>
+      <c r="BP18" s="8"/>
+      <c r="BQ18" s="8"/>
+      <c r="BR18" s="8"/>
+      <c r="BS18" s="8"/>
+      <c r="BT18" s="8"/>
+      <c r="BU18" s="8"/>
+      <c r="BV18" s="8"/>
+      <c r="BW18" s="8"/>
+      <c r="BX18" s="8"/>
+      <c r="BY18" s="8"/>
+      <c r="BZ18" s="8"/>
+      <c r="CA18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CB18" s="8"/>
+      <c r="CC18" s="8"/>
+      <c r="CD18" s="8"/>
+      <c r="CE18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+      <c r="CJ18" s="5"/>
+      <c r="CK18" s="5"/>
+      <c r="CL18" s="5"/>
+      <c r="CM18" s="5"/>
+      <c r="CN18" s="5"/>
+      <c r="CO18" s="5"/>
+      <c r="CP18" s="5"/>
+      <c r="CQ18" s="5"/>
+      <c r="CR18" s="5"/>
+      <c r="CS18" s="5"/>
+      <c r="CT18" s="5"/>
+      <c r="CU18" s="5"/>
+      <c r="CV18" s="5"/>
+      <c r="CW18" s="5"/>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1995,12 +2727,52 @@
       <c r="BI19" s="4"/>
       <c r="BJ19" s="4"/>
       <c r="BK19" s="4"/>
+      <c r="BL19" s="8"/>
+      <c r="BM19" s="8"/>
+      <c r="BN19" s="8"/>
+      <c r="BO19" s="8"/>
+      <c r="BP19" s="8"/>
+      <c r="BQ19" s="8"/>
+      <c r="BR19" s="8"/>
+      <c r="BS19" s="8"/>
+      <c r="BT19" s="8"/>
+      <c r="BU19" s="8"/>
+      <c r="BV19" s="8"/>
+      <c r="BW19" s="8"/>
+      <c r="BX19" s="8"/>
+      <c r="BY19" s="8"/>
+      <c r="BZ19" s="8"/>
+      <c r="CA19" s="8"/>
+      <c r="CB19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CC19" s="8"/>
+      <c r="CD19" s="8"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+      <c r="CK19" s="5"/>
+      <c r="CL19" s="5"/>
+      <c r="CM19" s="5"/>
+      <c r="CN19" s="5"/>
+      <c r="CO19" s="5"/>
+      <c r="CP19" s="5"/>
+      <c r="CQ19" s="5"/>
+      <c r="CR19" s="5"/>
+      <c r="CS19" s="5"/>
+      <c r="CT19" s="5"/>
+      <c r="CU19" s="5"/>
+      <c r="CV19" s="5"/>
+      <c r="CW19" s="5"/>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2064,12 +2836,52 @@
       </c>
       <c r="BJ20" s="4"/>
       <c r="BK20" s="4"/>
+      <c r="BL20" s="8"/>
+      <c r="BM20" s="8"/>
+      <c r="BN20" s="8"/>
+      <c r="BO20" s="8"/>
+      <c r="BP20" s="8"/>
+      <c r="BQ20" s="8"/>
+      <c r="BR20" s="8"/>
+      <c r="BS20" s="8"/>
+      <c r="BT20" s="8"/>
+      <c r="BU20" s="8"/>
+      <c r="BV20" s="8"/>
+      <c r="BW20" s="8"/>
+      <c r="BX20" s="8"/>
+      <c r="BY20" s="8"/>
+      <c r="BZ20" s="8"/>
+      <c r="CA20" s="8"/>
+      <c r="CB20" s="8"/>
+      <c r="CC20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CD20" s="8"/>
+      <c r="CE20" s="5"/>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+      <c r="CJ20" s="5"/>
+      <c r="CK20" s="5"/>
+      <c r="CL20" s="5"/>
+      <c r="CM20" s="5"/>
+      <c r="CN20" s="5"/>
+      <c r="CO20" s="5"/>
+      <c r="CP20" s="5"/>
+      <c r="CQ20" s="5"/>
+      <c r="CR20" s="5"/>
+      <c r="CS20" s="5"/>
+      <c r="CT20" s="5"/>
+      <c r="CU20" s="5"/>
+      <c r="CV20" s="5"/>
+      <c r="CW20" s="5"/>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2135,9 +2947,51 @@
       <c r="BK21" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="BL21" s="8"/>
+      <c r="BM21" s="8"/>
+      <c r="BN21" s="8"/>
+      <c r="BO21" s="8"/>
+      <c r="BP21" s="8"/>
+      <c r="BQ21" s="8"/>
+      <c r="BR21" s="8"/>
+      <c r="BS21" s="8"/>
+      <c r="BT21" s="8"/>
+      <c r="BU21" s="8"/>
+      <c r="BV21" s="8"/>
+      <c r="BW21" s="8"/>
+      <c r="BX21" s="8"/>
+      <c r="BY21" s="8"/>
+      <c r="BZ21" s="8"/>
+      <c r="CA21" s="8"/>
+      <c r="CB21" s="8"/>
+      <c r="CC21" s="8"/>
+      <c r="CD21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="CE21" s="5"/>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+      <c r="CJ21" s="5"/>
+      <c r="CK21" s="5"/>
+      <c r="CL21" s="5"/>
+      <c r="CM21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN21" s="5"/>
+      <c r="CO21" s="5"/>
+      <c r="CP21" s="5"/>
+      <c r="CQ21" s="5"/>
+      <c r="CR21" s="5"/>
+      <c r="CS21" s="5"/>
+      <c r="CT21" s="5"/>
+      <c r="CU21" s="5"/>
+      <c r="CV21" s="5"/>
+      <c r="CW21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -2154,9 +3008,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AQ2:BK2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -2165,6 +3016,11 @@
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="BL2:CD2"/>
+    <mergeCell ref="CE2:CW2"/>
+    <mergeCell ref="AQ2:BK2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert error in merging
</commit_message>
<xml_diff>
--- a/NC09_Matrice_di_tracciabilità.xlsx
+++ b/NC09_Matrice_di_tracciabilità.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B8F4D4-36BF-4693-BD41-3C72A33A6934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>Requisiti</t>
   </si>
@@ -229,12 +230,42 @@
   </si>
   <si>
     <t>Inventario</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Implementato</t>
+  </si>
+  <si>
+    <t>Sì</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>TC_C_1</t>
+  </si>
+  <si>
+    <t>TC_I_1</t>
+  </si>
+  <si>
+    <t>TC_A_1</t>
+  </si>
+  <si>
+    <t>TC_I_2</t>
+  </si>
+  <si>
+    <t>TC_U_1</t>
+  </si>
+  <si>
+    <t>TC_C_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -347,7 +378,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
@@ -362,6 +393,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,10 +406,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -660,16 +694,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AR4" sqref="AR4"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CN6" sqref="CN6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -678,28 +712,28 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="13"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
       <c r="P2" s="13" t="s">
         <v>35</v>
       </c>
@@ -735,35 +769,77 @@
       <c r="AN2" s="13"/>
       <c r="AO2" s="13"/>
       <c r="AP2" s="13"/>
-      <c r="AQ2" s="8" t="s">
+      <c r="AQ2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="9"/>
-      <c r="AY2" s="9"/>
-      <c r="AZ2" s="9"/>
-      <c r="BA2" s="9"/>
-      <c r="BB2" s="9"/>
-      <c r="BC2" s="9"/>
-      <c r="BD2" s="9"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="9"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="9"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="9"/>
-      <c r="BK2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
+      <c r="BO2" s="10"/>
+      <c r="BP2" s="10"/>
+      <c r="BQ2" s="10"/>
+      <c r="BR2" s="10"/>
+      <c r="BS2" s="10"/>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="10"/>
+      <c r="BV2" s="10"/>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10"/>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="CF2" s="10"/>
+      <c r="CG2" s="10"/>
+      <c r="CH2" s="10"/>
+      <c r="CI2" s="10"/>
+      <c r="CJ2" s="10"/>
+      <c r="CK2" s="10"/>
+      <c r="CL2" s="10"/>
+      <c r="CM2" s="10"/>
+      <c r="CN2" s="10"/>
+      <c r="CO2" s="10"/>
+      <c r="CP2" s="10"/>
+      <c r="CQ2" s="10"/>
+      <c r="CR2" s="10"/>
+      <c r="CS2" s="10"/>
+      <c r="CT2" s="10"/>
+      <c r="CU2" s="10"/>
+      <c r="CV2" s="10"/>
+      <c r="CW2" s="10"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -829,12 +905,54 @@
       <c r="BI3" s="4"/>
       <c r="BJ3" s="4"/>
       <c r="BK3" s="4"/>
+      <c r="BL3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CE3" s="5"/>
+      <c r="CF3" s="5"/>
+      <c r="CG3" s="5"/>
+      <c r="CH3" s="5"/>
+      <c r="CI3" s="5"/>
+      <c r="CJ3" s="5"/>
+      <c r="CK3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL3" s="5"/>
+      <c r="CM3" s="5"/>
+      <c r="CN3" s="5"/>
+      <c r="CO3" s="5"/>
+      <c r="CP3" s="5"/>
+      <c r="CQ3" s="5"/>
+      <c r="CR3" s="5"/>
+      <c r="CS3" s="5"/>
+      <c r="CT3" s="5"/>
+      <c r="CU3" s="5"/>
+      <c r="CV3" s="5"/>
+      <c r="CW3" s="5"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -896,12 +1014,52 @@
       <c r="BI4" s="4"/>
       <c r="BJ4" s="4"/>
       <c r="BK4" s="4"/>
+      <c r="BL4" s="8"/>
+      <c r="BM4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN4" s="8"/>
+      <c r="BO4" s="8"/>
+      <c r="BP4" s="8"/>
+      <c r="BQ4" s="8"/>
+      <c r="BR4" s="8"/>
+      <c r="BS4" s="8"/>
+      <c r="BT4" s="8"/>
+      <c r="BU4" s="8"/>
+      <c r="BV4" s="8"/>
+      <c r="BW4" s="8"/>
+      <c r="BX4" s="8"/>
+      <c r="BY4" s="8"/>
+      <c r="BZ4" s="8"/>
+      <c r="CA4" s="8"/>
+      <c r="CB4" s="8"/>
+      <c r="CC4" s="8"/>
+      <c r="CD4" s="8"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+      <c r="CK4" s="5"/>
+      <c r="CL4" s="5"/>
+      <c r="CM4" s="5"/>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
@@ -977,12 +1135,54 @@
       <c r="BI5" s="4"/>
       <c r="BJ5" s="4"/>
       <c r="BK5" s="4"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO5" s="8"/>
+      <c r="BP5" s="8"/>
+      <c r="BQ5" s="8"/>
+      <c r="BR5" s="8"/>
+      <c r="BS5" s="8"/>
+      <c r="BT5" s="8"/>
+      <c r="BU5" s="8"/>
+      <c r="BV5" s="8"/>
+      <c r="BW5" s="8"/>
+      <c r="BX5" s="8"/>
+      <c r="BY5" s="8"/>
+      <c r="BZ5" s="8"/>
+      <c r="CA5" s="8"/>
+      <c r="CB5" s="8"/>
+      <c r="CC5" s="8"/>
+      <c r="CD5" s="8"/>
+      <c r="CE5" s="5"/>
+      <c r="CF5" s="5"/>
+      <c r="CG5" s="5"/>
+      <c r="CH5" s="5"/>
+      <c r="CI5" s="5"/>
+      <c r="CJ5" s="5"/>
+      <c r="CK5" s="5"/>
+      <c r="CL5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM5" s="5"/>
+      <c r="CN5" s="5"/>
+      <c r="CO5" s="5"/>
+      <c r="CP5" s="5"/>
+      <c r="CQ5" s="5"/>
+      <c r="CR5" s="5"/>
+      <c r="CS5" s="5"/>
+      <c r="CT5" s="5"/>
+      <c r="CU5" s="5"/>
+      <c r="CV5" s="5"/>
+      <c r="CW5" s="5"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1046,12 +1246,52 @@
       <c r="BI6" s="4"/>
       <c r="BJ6" s="4"/>
       <c r="BK6" s="4"/>
+      <c r="BL6" s="8"/>
+      <c r="BM6" s="8"/>
+      <c r="BN6" s="8"/>
+      <c r="BO6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BP6" s="8"/>
+      <c r="BQ6" s="8"/>
+      <c r="BR6" s="8"/>
+      <c r="BS6" s="8"/>
+      <c r="BT6" s="8"/>
+      <c r="BU6" s="8"/>
+      <c r="BV6" s="8"/>
+      <c r="BW6" s="8"/>
+      <c r="BX6" s="8"/>
+      <c r="BY6" s="8"/>
+      <c r="BZ6" s="8"/>
+      <c r="CA6" s="8"/>
+      <c r="CB6" s="8"/>
+      <c r="CC6" s="8"/>
+      <c r="CD6" s="8"/>
+      <c r="CE6" s="5"/>
+      <c r="CF6" s="5"/>
+      <c r="CG6" s="5"/>
+      <c r="CH6" s="5"/>
+      <c r="CI6" s="5"/>
+      <c r="CJ6" s="5"/>
+      <c r="CK6" s="5"/>
+      <c r="CL6" s="5"/>
+      <c r="CM6" s="5"/>
+      <c r="CN6" s="5"/>
+      <c r="CO6" s="5"/>
+      <c r="CP6" s="5"/>
+      <c r="CQ6" s="5"/>
+      <c r="CR6" s="5"/>
+      <c r="CS6" s="5"/>
+      <c r="CT6" s="5"/>
+      <c r="CU6" s="5"/>
+      <c r="CV6" s="5"/>
+      <c r="CW6" s="5"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1117,12 +1357,54 @@
       <c r="BI7" s="4"/>
       <c r="BJ7" s="4"/>
       <c r="BK7" s="4"/>
+      <c r="BL7" s="8"/>
+      <c r="BM7" s="8"/>
+      <c r="BN7" s="8"/>
+      <c r="BO7" s="8"/>
+      <c r="BP7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ7" s="8"/>
+      <c r="BR7" s="8"/>
+      <c r="BS7" s="8"/>
+      <c r="BT7" s="8"/>
+      <c r="BU7" s="8"/>
+      <c r="BV7" s="8"/>
+      <c r="BW7" s="8"/>
+      <c r="BX7" s="8"/>
+      <c r="BY7" s="8"/>
+      <c r="BZ7" s="8"/>
+      <c r="CA7" s="8"/>
+      <c r="CB7" s="8"/>
+      <c r="CC7" s="8"/>
+      <c r="CD7" s="8"/>
+      <c r="CE7" s="5"/>
+      <c r="CF7" s="5"/>
+      <c r="CG7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CH7" s="5"/>
+      <c r="CI7" s="5"/>
+      <c r="CJ7" s="5"/>
+      <c r="CK7" s="5"/>
+      <c r="CL7" s="5"/>
+      <c r="CM7" s="5"/>
+      <c r="CN7" s="5"/>
+      <c r="CO7" s="5"/>
+      <c r="CP7" s="5"/>
+      <c r="CQ7" s="5"/>
+      <c r="CR7" s="5"/>
+      <c r="CS7" s="5"/>
+      <c r="CT7" s="5"/>
+      <c r="CU7" s="5"/>
+      <c r="CV7" s="5"/>
+      <c r="CW7" s="5"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1186,12 +1468,54 @@
       <c r="BI8" s="4"/>
       <c r="BJ8" s="4"/>
       <c r="BK8" s="4"/>
+      <c r="BL8" s="8"/>
+      <c r="BM8" s="8"/>
+      <c r="BN8" s="8"/>
+      <c r="BO8" s="8"/>
+      <c r="BP8" s="8"/>
+      <c r="BQ8" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR8" s="8"/>
+      <c r="BS8" s="8"/>
+      <c r="BT8" s="8"/>
+      <c r="BU8" s="8"/>
+      <c r="BV8" s="8"/>
+      <c r="BW8" s="8"/>
+      <c r="BX8" s="8"/>
+      <c r="BY8" s="8"/>
+      <c r="BZ8" s="8"/>
+      <c r="CA8" s="8"/>
+      <c r="CB8" s="8"/>
+      <c r="CC8" s="8"/>
+      <c r="CD8" s="8"/>
+      <c r="CE8" s="5"/>
+      <c r="CF8" s="5"/>
+      <c r="CG8" s="5"/>
+      <c r="CH8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI8" s="5"/>
+      <c r="CJ8" s="5"/>
+      <c r="CK8" s="5"/>
+      <c r="CL8" s="5"/>
+      <c r="CM8" s="5"/>
+      <c r="CN8" s="5"/>
+      <c r="CO8" s="5"/>
+      <c r="CP8" s="5"/>
+      <c r="CQ8" s="5"/>
+      <c r="CR8" s="5"/>
+      <c r="CS8" s="5"/>
+      <c r="CT8" s="5"/>
+      <c r="CU8" s="5"/>
+      <c r="CV8" s="5"/>
+      <c r="CW8" s="5"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5" t="s">
         <v>22</v>
@@ -1259,12 +1583,54 @@
       <c r="BI9" s="4"/>
       <c r="BJ9" s="4"/>
       <c r="BK9" s="4"/>
+      <c r="BL9" s="8"/>
+      <c r="BM9" s="8"/>
+      <c r="BN9" s="8"/>
+      <c r="BO9" s="8"/>
+      <c r="BP9" s="8"/>
+      <c r="BQ9" s="8"/>
+      <c r="BR9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS9" s="8"/>
+      <c r="BT9" s="8"/>
+      <c r="BU9" s="8"/>
+      <c r="BV9" s="8"/>
+      <c r="BW9" s="8"/>
+      <c r="BX9" s="8"/>
+      <c r="BY9" s="8"/>
+      <c r="BZ9" s="8"/>
+      <c r="CA9" s="8"/>
+      <c r="CB9" s="8"/>
+      <c r="CC9" s="8"/>
+      <c r="CD9" s="8"/>
+      <c r="CE9" s="5"/>
+      <c r="CF9" s="5"/>
+      <c r="CG9" s="5"/>
+      <c r="CH9" s="5"/>
+      <c r="CI9" s="5"/>
+      <c r="CJ9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="CK9" s="5"/>
+      <c r="CL9" s="5"/>
+      <c r="CM9" s="5"/>
+      <c r="CN9" s="5"/>
+      <c r="CO9" s="5"/>
+      <c r="CP9" s="5"/>
+      <c r="CQ9" s="5"/>
+      <c r="CR9" s="5"/>
+      <c r="CS9" s="5"/>
+      <c r="CT9" s="5"/>
+      <c r="CU9" s="5"/>
+      <c r="CV9" s="5"/>
+      <c r="CW9" s="5"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1326,12 +1692,52 @@
       <c r="BI10" s="4"/>
       <c r="BJ10" s="4"/>
       <c r="BK10" s="4"/>
+      <c r="BL10" s="8"/>
+      <c r="BM10" s="8"/>
+      <c r="BN10" s="8"/>
+      <c r="BO10" s="8"/>
+      <c r="BP10" s="8"/>
+      <c r="BQ10" s="8"/>
+      <c r="BR10" s="8"/>
+      <c r="BS10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BT10" s="8"/>
+      <c r="BU10" s="8"/>
+      <c r="BV10" s="8"/>
+      <c r="BW10" s="8"/>
+      <c r="BX10" s="8"/>
+      <c r="BY10" s="8"/>
+      <c r="BZ10" s="8"/>
+      <c r="CA10" s="8"/>
+      <c r="CB10" s="8"/>
+      <c r="CC10" s="8"/>
+      <c r="CD10" s="8"/>
+      <c r="CE10" s="5"/>
+      <c r="CF10" s="5"/>
+      <c r="CG10" s="5"/>
+      <c r="CH10" s="5"/>
+      <c r="CI10" s="5"/>
+      <c r="CJ10" s="5"/>
+      <c r="CK10" s="5"/>
+      <c r="CL10" s="5"/>
+      <c r="CM10" s="5"/>
+      <c r="CN10" s="5"/>
+      <c r="CO10" s="5"/>
+      <c r="CP10" s="5"/>
+      <c r="CQ10" s="5"/>
+      <c r="CR10" s="5"/>
+      <c r="CS10" s="5"/>
+      <c r="CT10" s="5"/>
+      <c r="CU10" s="5"/>
+      <c r="CV10" s="5"/>
+      <c r="CW10" s="5"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1393,12 +1799,52 @@
       <c r="BI11" s="4"/>
       <c r="BJ11" s="4"/>
       <c r="BK11" s="4"/>
+      <c r="BL11" s="8"/>
+      <c r="BM11" s="8"/>
+      <c r="BN11" s="8"/>
+      <c r="BO11" s="8"/>
+      <c r="BP11" s="8"/>
+      <c r="BQ11" s="8"/>
+      <c r="BR11" s="8"/>
+      <c r="BS11" s="8"/>
+      <c r="BT11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU11" s="8"/>
+      <c r="BV11" s="8"/>
+      <c r="BW11" s="8"/>
+      <c r="BX11" s="8"/>
+      <c r="BY11" s="8"/>
+      <c r="BZ11" s="8"/>
+      <c r="CA11" s="8"/>
+      <c r="CB11" s="8"/>
+      <c r="CC11" s="8"/>
+      <c r="CD11" s="8"/>
+      <c r="CE11" s="5"/>
+      <c r="CF11" s="5"/>
+      <c r="CG11" s="5"/>
+      <c r="CH11" s="5"/>
+      <c r="CI11" s="5"/>
+      <c r="CJ11" s="5"/>
+      <c r="CK11" s="5"/>
+      <c r="CL11" s="5"/>
+      <c r="CM11" s="5"/>
+      <c r="CN11" s="5"/>
+      <c r="CO11" s="5"/>
+      <c r="CP11" s="5"/>
+      <c r="CQ11" s="5"/>
+      <c r="CR11" s="5"/>
+      <c r="CS11" s="5"/>
+      <c r="CT11" s="5"/>
+      <c r="CU11" s="5"/>
+      <c r="CV11" s="5"/>
+      <c r="CW11" s="5"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1462,12 +1908,52 @@
       <c r="BI12" s="4"/>
       <c r="BJ12" s="4"/>
       <c r="BK12" s="4"/>
+      <c r="BL12" s="8"/>
+      <c r="BM12" s="8"/>
+      <c r="BN12" s="8"/>
+      <c r="BO12" s="8"/>
+      <c r="BP12" s="8"/>
+      <c r="BQ12" s="8"/>
+      <c r="BR12" s="8"/>
+      <c r="BS12" s="8"/>
+      <c r="BT12" s="8"/>
+      <c r="BU12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV12" s="8"/>
+      <c r="BW12" s="8"/>
+      <c r="BX12" s="8"/>
+      <c r="BY12" s="8"/>
+      <c r="BZ12" s="8"/>
+      <c r="CA12" s="8"/>
+      <c r="CB12" s="8"/>
+      <c r="CC12" s="8"/>
+      <c r="CD12" s="8"/>
+      <c r="CE12" s="5"/>
+      <c r="CF12" s="5"/>
+      <c r="CG12" s="5"/>
+      <c r="CH12" s="5"/>
+      <c r="CI12" s="5"/>
+      <c r="CJ12" s="5"/>
+      <c r="CK12" s="5"/>
+      <c r="CL12" s="5"/>
+      <c r="CM12" s="5"/>
+      <c r="CN12" s="5"/>
+      <c r="CO12" s="5"/>
+      <c r="CP12" s="5"/>
+      <c r="CQ12" s="5"/>
+      <c r="CR12" s="5"/>
+      <c r="CS12" s="5"/>
+      <c r="CT12" s="5"/>
+      <c r="CU12" s="5"/>
+      <c r="CV12" s="5"/>
+      <c r="CW12" s="5"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5" t="s">
@@ -1541,12 +2027,54 @@
       <c r="BI13" s="4"/>
       <c r="BJ13" s="4"/>
       <c r="BK13" s="4"/>
+      <c r="BL13" s="8"/>
+      <c r="BM13" s="8"/>
+      <c r="BN13" s="8"/>
+      <c r="BO13" s="8"/>
+      <c r="BP13" s="8"/>
+      <c r="BQ13" s="8"/>
+      <c r="BR13" s="8"/>
+      <c r="BS13" s="8"/>
+      <c r="BT13" s="8"/>
+      <c r="BU13" s="8"/>
+      <c r="BV13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW13" s="8"/>
+      <c r="BX13" s="8"/>
+      <c r="BY13" s="8"/>
+      <c r="BZ13" s="8"/>
+      <c r="CA13" s="8"/>
+      <c r="CB13" s="8"/>
+      <c r="CC13" s="8"/>
+      <c r="CD13" s="8"/>
+      <c r="CE13" s="5"/>
+      <c r="CF13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="CG13" s="5"/>
+      <c r="CH13" s="5"/>
+      <c r="CI13" s="5"/>
+      <c r="CJ13" s="5"/>
+      <c r="CK13" s="5"/>
+      <c r="CL13" s="5"/>
+      <c r="CM13" s="5"/>
+      <c r="CN13" s="5"/>
+      <c r="CO13" s="5"/>
+      <c r="CP13" s="5"/>
+      <c r="CQ13" s="5"/>
+      <c r="CR13" s="5"/>
+      <c r="CS13" s="5"/>
+      <c r="CT13" s="5"/>
+      <c r="CU13" s="5"/>
+      <c r="CV13" s="5"/>
+      <c r="CW13" s="5"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1620,12 +2148,54 @@
       <c r="BI14" s="4"/>
       <c r="BJ14" s="4"/>
       <c r="BK14" s="4"/>
+      <c r="BL14" s="8"/>
+      <c r="BM14" s="8"/>
+      <c r="BN14" s="8"/>
+      <c r="BO14" s="8"/>
+      <c r="BP14" s="8"/>
+      <c r="BQ14" s="8"/>
+      <c r="BR14" s="8"/>
+      <c r="BS14" s="8"/>
+      <c r="BT14" s="8"/>
+      <c r="BU14" s="8"/>
+      <c r="BV14" s="8"/>
+      <c r="BW14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BX14" s="8"/>
+      <c r="BY14" s="8"/>
+      <c r="BZ14" s="8"/>
+      <c r="CA14" s="8"/>
+      <c r="CB14" s="8"/>
+      <c r="CC14" s="8"/>
+      <c r="CD14" s="8"/>
+      <c r="CE14" s="5"/>
+      <c r="CF14" s="5"/>
+      <c r="CG14" s="5"/>
+      <c r="CH14" s="5"/>
+      <c r="CI14" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="CJ14" s="5"/>
+      <c r="CK14" s="5"/>
+      <c r="CL14" s="5"/>
+      <c r="CM14" s="5"/>
+      <c r="CN14" s="5"/>
+      <c r="CO14" s="5"/>
+      <c r="CP14" s="5"/>
+      <c r="CQ14" s="5"/>
+      <c r="CR14" s="5"/>
+      <c r="CS14" s="5"/>
+      <c r="CT14" s="5"/>
+      <c r="CU14" s="5"/>
+      <c r="CV14" s="5"/>
+      <c r="CW14" s="5"/>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1687,12 +2257,52 @@
       <c r="BI15" s="4"/>
       <c r="BJ15" s="4"/>
       <c r="BK15" s="4"/>
+      <c r="BL15" s="8"/>
+      <c r="BM15" s="8"/>
+      <c r="BN15" s="8"/>
+      <c r="BO15" s="8"/>
+      <c r="BP15" s="8"/>
+      <c r="BQ15" s="8"/>
+      <c r="BR15" s="8"/>
+      <c r="BS15" s="8"/>
+      <c r="BT15" s="8"/>
+      <c r="BU15" s="8"/>
+      <c r="BV15" s="8"/>
+      <c r="BW15" s="8"/>
+      <c r="BX15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="BY15" s="8"/>
+      <c r="BZ15" s="8"/>
+      <c r="CA15" s="8"/>
+      <c r="CB15" s="8"/>
+      <c r="CC15" s="8"/>
+      <c r="CD15" s="8"/>
+      <c r="CE15" s="5"/>
+      <c r="CF15" s="5"/>
+      <c r="CG15" s="5"/>
+      <c r="CH15" s="5"/>
+      <c r="CI15" s="5"/>
+      <c r="CJ15" s="5"/>
+      <c r="CK15" s="5"/>
+      <c r="CL15" s="5"/>
+      <c r="CM15" s="5"/>
+      <c r="CN15" s="5"/>
+      <c r="CO15" s="5"/>
+      <c r="CP15" s="5"/>
+      <c r="CQ15" s="5"/>
+      <c r="CR15" s="5"/>
+      <c r="CS15" s="5"/>
+      <c r="CT15" s="5"/>
+      <c r="CU15" s="5"/>
+      <c r="CV15" s="5"/>
+      <c r="CW15" s="5"/>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1766,12 +2376,52 @@
       <c r="BI16" s="4"/>
       <c r="BJ16" s="4"/>
       <c r="BK16" s="4"/>
+      <c r="BL16" s="8"/>
+      <c r="BM16" s="8"/>
+      <c r="BN16" s="8"/>
+      <c r="BO16" s="8"/>
+      <c r="BP16" s="8"/>
+      <c r="BQ16" s="8"/>
+      <c r="BR16" s="8"/>
+      <c r="BS16" s="8"/>
+      <c r="BT16" s="8"/>
+      <c r="BU16" s="8"/>
+      <c r="BV16" s="8"/>
+      <c r="BW16" s="8"/>
+      <c r="BX16" s="8"/>
+      <c r="BY16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="BZ16" s="8"/>
+      <c r="CA16" s="8"/>
+      <c r="CB16" s="8"/>
+      <c r="CC16" s="8"/>
+      <c r="CD16" s="8"/>
+      <c r="CE16" s="5"/>
+      <c r="CF16" s="5"/>
+      <c r="CG16" s="5"/>
+      <c r="CH16" s="5"/>
+      <c r="CI16" s="5"/>
+      <c r="CJ16" s="5"/>
+      <c r="CK16" s="5"/>
+      <c r="CL16" s="5"/>
+      <c r="CM16" s="5"/>
+      <c r="CN16" s="5"/>
+      <c r="CO16" s="5"/>
+      <c r="CP16" s="5"/>
+      <c r="CQ16" s="5"/>
+      <c r="CR16" s="5"/>
+      <c r="CS16" s="5"/>
+      <c r="CT16" s="5"/>
+      <c r="CU16" s="5"/>
+      <c r="CV16" s="5"/>
+      <c r="CW16" s="5"/>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1845,12 +2495,52 @@
       <c r="BI17" s="4"/>
       <c r="BJ17" s="4"/>
       <c r="BK17" s="4"/>
+      <c r="BL17" s="8"/>
+      <c r="BM17" s="8"/>
+      <c r="BN17" s="8"/>
+      <c r="BO17" s="8"/>
+      <c r="BP17" s="8"/>
+      <c r="BQ17" s="8"/>
+      <c r="BR17" s="8"/>
+      <c r="BS17" s="8"/>
+      <c r="BT17" s="8"/>
+      <c r="BU17" s="8"/>
+      <c r="BV17" s="8"/>
+      <c r="BW17" s="8"/>
+      <c r="BX17" s="8"/>
+      <c r="BY17" s="8"/>
+      <c r="BZ17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CA17" s="8"/>
+      <c r="CB17" s="8"/>
+      <c r="CC17" s="8"/>
+      <c r="CD17" s="8"/>
+      <c r="CE17" s="5"/>
+      <c r="CF17" s="5"/>
+      <c r="CG17" s="5"/>
+      <c r="CH17" s="5"/>
+      <c r="CI17" s="5"/>
+      <c r="CJ17" s="5"/>
+      <c r="CK17" s="5"/>
+      <c r="CL17" s="5"/>
+      <c r="CM17" s="5"/>
+      <c r="CN17" s="5"/>
+      <c r="CO17" s="5"/>
+      <c r="CP17" s="5"/>
+      <c r="CQ17" s="5"/>
+      <c r="CR17" s="5"/>
+      <c r="CS17" s="5"/>
+      <c r="CT17" s="5"/>
+      <c r="CU17" s="5"/>
+      <c r="CV17" s="5"/>
+      <c r="CW17" s="5"/>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1924,12 +2614,54 @@
       <c r="BI18" s="4"/>
       <c r="BJ18" s="4"/>
       <c r="BK18" s="4"/>
+      <c r="BL18" s="8"/>
+      <c r="BM18" s="8"/>
+      <c r="BN18" s="8"/>
+      <c r="BO18" s="8"/>
+      <c r="BP18" s="8"/>
+      <c r="BQ18" s="8"/>
+      <c r="BR18" s="8"/>
+      <c r="BS18" s="8"/>
+      <c r="BT18" s="8"/>
+      <c r="BU18" s="8"/>
+      <c r="BV18" s="8"/>
+      <c r="BW18" s="8"/>
+      <c r="BX18" s="8"/>
+      <c r="BY18" s="8"/>
+      <c r="BZ18" s="8"/>
+      <c r="CA18" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CB18" s="8"/>
+      <c r="CC18" s="8"/>
+      <c r="CD18" s="8"/>
+      <c r="CE18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CF18" s="5"/>
+      <c r="CG18" s="5"/>
+      <c r="CH18" s="5"/>
+      <c r="CI18" s="5"/>
+      <c r="CJ18" s="5"/>
+      <c r="CK18" s="5"/>
+      <c r="CL18" s="5"/>
+      <c r="CM18" s="5"/>
+      <c r="CN18" s="5"/>
+      <c r="CO18" s="5"/>
+      <c r="CP18" s="5"/>
+      <c r="CQ18" s="5"/>
+      <c r="CR18" s="5"/>
+      <c r="CS18" s="5"/>
+      <c r="CT18" s="5"/>
+      <c r="CU18" s="5"/>
+      <c r="CV18" s="5"/>
+      <c r="CW18" s="5"/>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1995,12 +2727,52 @@
       <c r="BI19" s="4"/>
       <c r="BJ19" s="4"/>
       <c r="BK19" s="4"/>
+      <c r="BL19" s="8"/>
+      <c r="BM19" s="8"/>
+      <c r="BN19" s="8"/>
+      <c r="BO19" s="8"/>
+      <c r="BP19" s="8"/>
+      <c r="BQ19" s="8"/>
+      <c r="BR19" s="8"/>
+      <c r="BS19" s="8"/>
+      <c r="BT19" s="8"/>
+      <c r="BU19" s="8"/>
+      <c r="BV19" s="8"/>
+      <c r="BW19" s="8"/>
+      <c r="BX19" s="8"/>
+      <c r="BY19" s="8"/>
+      <c r="BZ19" s="8"/>
+      <c r="CA19" s="8"/>
+      <c r="CB19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CC19" s="8"/>
+      <c r="CD19" s="8"/>
+      <c r="CE19" s="5"/>
+      <c r="CF19" s="5"/>
+      <c r="CG19" s="5"/>
+      <c r="CH19" s="5"/>
+      <c r="CI19" s="5"/>
+      <c r="CJ19" s="5"/>
+      <c r="CK19" s="5"/>
+      <c r="CL19" s="5"/>
+      <c r="CM19" s="5"/>
+      <c r="CN19" s="5"/>
+      <c r="CO19" s="5"/>
+      <c r="CP19" s="5"/>
+      <c r="CQ19" s="5"/>
+      <c r="CR19" s="5"/>
+      <c r="CS19" s="5"/>
+      <c r="CT19" s="5"/>
+      <c r="CU19" s="5"/>
+      <c r="CV19" s="5"/>
+      <c r="CW19" s="5"/>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -2064,12 +2836,52 @@
       </c>
       <c r="BJ20" s="4"/>
       <c r="BK20" s="4"/>
+      <c r="BL20" s="8"/>
+      <c r="BM20" s="8"/>
+      <c r="BN20" s="8"/>
+      <c r="BO20" s="8"/>
+      <c r="BP20" s="8"/>
+      <c r="BQ20" s="8"/>
+      <c r="BR20" s="8"/>
+      <c r="BS20" s="8"/>
+      <c r="BT20" s="8"/>
+      <c r="BU20" s="8"/>
+      <c r="BV20" s="8"/>
+      <c r="BW20" s="8"/>
+      <c r="BX20" s="8"/>
+      <c r="BY20" s="8"/>
+      <c r="BZ20" s="8"/>
+      <c r="CA20" s="8"/>
+      <c r="CB20" s="8"/>
+      <c r="CC20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="CD20" s="8"/>
+      <c r="CE20" s="5"/>
+      <c r="CF20" s="5"/>
+      <c r="CG20" s="5"/>
+      <c r="CH20" s="5"/>
+      <c r="CI20" s="5"/>
+      <c r="CJ20" s="5"/>
+      <c r="CK20" s="5"/>
+      <c r="CL20" s="5"/>
+      <c r="CM20" s="5"/>
+      <c r="CN20" s="5"/>
+      <c r="CO20" s="5"/>
+      <c r="CP20" s="5"/>
+      <c r="CQ20" s="5"/>
+      <c r="CR20" s="5"/>
+      <c r="CS20" s="5"/>
+      <c r="CT20" s="5"/>
+      <c r="CU20" s="5"/>
+      <c r="CV20" s="5"/>
+      <c r="CW20" s="5"/>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -2135,9 +2947,51 @@
       <c r="BK21" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="BL21" s="8"/>
+      <c r="BM21" s="8"/>
+      <c r="BN21" s="8"/>
+      <c r="BO21" s="8"/>
+      <c r="BP21" s="8"/>
+      <c r="BQ21" s="8"/>
+      <c r="BR21" s="8"/>
+      <c r="BS21" s="8"/>
+      <c r="BT21" s="8"/>
+      <c r="BU21" s="8"/>
+      <c r="BV21" s="8"/>
+      <c r="BW21" s="8"/>
+      <c r="BX21" s="8"/>
+      <c r="BY21" s="8"/>
+      <c r="BZ21" s="8"/>
+      <c r="CA21" s="8"/>
+      <c r="CB21" s="8"/>
+      <c r="CC21" s="8"/>
+      <c r="CD21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="CE21" s="5"/>
+      <c r="CF21" s="5"/>
+      <c r="CG21" s="5"/>
+      <c r="CH21" s="5"/>
+      <c r="CI21" s="5"/>
+      <c r="CJ21" s="5"/>
+      <c r="CK21" s="5"/>
+      <c r="CL21" s="5"/>
+      <c r="CM21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN21" s="5"/>
+      <c r="CO21" s="5"/>
+      <c r="CP21" s="5"/>
+      <c r="CQ21" s="5"/>
+      <c r="CR21" s="5"/>
+      <c r="CS21" s="5"/>
+      <c r="CT21" s="5"/>
+      <c r="CU21" s="5"/>
+      <c r="CV21" s="5"/>
+      <c r="CW21" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="29">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -2154,9 +3008,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="AQ2:BK2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:B2"/>
@@ -2165,6 +3016,11 @@
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:AA2"/>
+    <mergeCell ref="BL2:CD2"/>
+    <mergeCell ref="CE2:CW2"/>
+    <mergeCell ref="AQ2:BK2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>